<commit_message>
Ball - Yang - Analysis: distribution vs working distance
yang
- tried to look at ray distribution on detector changing as it changes
with increasing working distance, analyzed data for chan=25 case with
bare channel

- lensless: finished processing xslx contents
- ignore figures and tempfiles for github
</commit_message>
<xml_diff>
--- a/Geometry/Ball/Papers/yang.xlsx
+++ b/Geometry/Ball/Papers/yang.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Dropbox\simulation\geometry\ball\papers\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Dropbox\Simulation\Geometry\Ball\Papers\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="25">
   <si>
     <t xml:space="preserve"> lens half submerged in channel medium above channel</t>
   </si>
@@ -95,6 +95,9 @@
   </si>
   <si>
     <t>SIM 2: lens half submerged in channel medium above channel, reflecting coating on well and channel, different reflective coatings, thin pdms over well</t>
+  </si>
+  <si>
+    <t>DISTRIBUTION</t>
   </si>
 </sst>
 </file>
@@ -702,6 +705,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -808,11 +812,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="50887568"/>
-        <c:axId val="50887008"/>
+        <c:axId val="156019904"/>
+        <c:axId val="156020464"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="50887568"/>
+        <c:axId val="156019904"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -869,12 +873,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="50887008"/>
+        <c:crossAx val="156020464"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="50887008"/>
+        <c:axId val="156020464"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -931,7 +935,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="50887568"/>
+        <c:crossAx val="156019904"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1039,6 +1043,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -1147,11 +1152,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="333010400"/>
-        <c:axId val="333008160"/>
+        <c:axId val="156022704"/>
+        <c:axId val="156023264"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="333010400"/>
+        <c:axId val="156022704"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1208,12 +1213,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="333008160"/>
+        <c:crossAx val="156023264"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="333008160"/>
+        <c:axId val="156023264"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1270,7 +1275,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="333010400"/>
+        <c:crossAx val="156022704"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2759,10 +2764,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:O541"/>
+  <dimension ref="A1:P537"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A473" workbookViewId="0">
-      <selection activeCell="P359" sqref="P359"/>
+    <sheetView tabSelected="1" topLeftCell="A464" workbookViewId="0">
+      <selection activeCell="M492" sqref="M492:P492"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -22609,7 +22614,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="449" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="449" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A449">
         <v>0.59</v>
       </c>
@@ -22656,7 +22661,7 @@
         <v>5.5003994790000003E-2</v>
       </c>
     </row>
-    <row r="450" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="450" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A450">
         <v>0.59</v>
       </c>
@@ -22703,7 +22708,7 @@
         <v>5.9078364770000003E-2</v>
       </c>
     </row>
-    <row r="451" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="451" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A451">
         <v>0.59</v>
       </c>
@@ -22750,7 +22755,7 @@
         <v>4.6402547039999999E-2</v>
       </c>
     </row>
-    <row r="452" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="452" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A452">
         <v>0.59</v>
       </c>
@@ -22797,7 +22802,7 @@
         <v>4.2016940459999999E-2</v>
       </c>
     </row>
-    <row r="453" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="453" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A453">
         <v>0.59</v>
       </c>
@@ -22844,7 +22849,7 @@
         <v>2.9335463879999999E-2</v>
       </c>
     </row>
-    <row r="454" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="454" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A454">
         <v>0.59</v>
       </c>
@@ -22891,7 +22896,7 @@
         <v>2.0711380750000001E-2</v>
       </c>
     </row>
-    <row r="455" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="455" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A455" t="s">
         <v>20</v>
       </c>
@@ -22899,7 +22904,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="456" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="456" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A456" t="s">
         <v>1</v>
       </c>
@@ -22945,8 +22950,11 @@
       <c r="O456" s="4" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="457" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P456" s="4" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="457" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A457">
         <v>0.59</v>
       </c>
@@ -22974,7 +22982,7 @@
       <c r="I457">
         <v>25</v>
       </c>
-      <c r="J457">
+      <c r="J457" s="1">
         <v>0</v>
       </c>
       <c r="K457">
@@ -22983,17 +22991,21 @@
       <c r="L457">
         <v>25</v>
       </c>
-      <c r="M457">
+      <c r="M457" s="1">
         <v>12.5</v>
       </c>
-      <c r="N457">
+      <c r="N457" s="1">
         <v>27</v>
       </c>
-      <c r="O457">
+      <c r="O457" s="1">
         <v>5.5003994790000003E-2</v>
       </c>
-    </row>
-    <row r="458" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P457" s="1">
+        <f>O457</f>
+        <v>5.5003994790000003E-2</v>
+      </c>
+    </row>
+    <row r="458" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A458">
         <v>0.59</v>
       </c>
@@ -23021,7 +23033,7 @@
       <c r="I458">
         <v>25</v>
       </c>
-      <c r="J458">
+      <c r="J458" s="1">
         <v>0</v>
       </c>
       <c r="K458">
@@ -23030,17 +23042,21 @@
       <c r="L458">
         <v>25</v>
       </c>
-      <c r="M458">
-        <v>25</v>
-      </c>
-      <c r="N458">
+      <c r="M458" s="1">
+        <v>25</v>
+      </c>
+      <c r="N458" s="1">
         <v>116</v>
       </c>
-      <c r="O458">
+      <c r="O458" s="1">
         <v>5.9078364770000003E-2</v>
       </c>
-    </row>
-    <row r="459" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P458" s="1">
+        <f>(N458-N457)/(PI()*(M458^2-M457^2))</f>
+        <v>6.0436437056762389E-2</v>
+      </c>
+    </row>
+    <row r="459" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A459">
         <v>0.59</v>
       </c>
@@ -23068,7 +23084,7 @@
       <c r="I459">
         <v>25</v>
       </c>
-      <c r="J459">
+      <c r="J459" s="1">
         <v>0</v>
       </c>
       <c r="K459">
@@ -23077,17 +23093,21 @@
       <c r="L459">
         <v>25</v>
       </c>
-      <c r="M459">
+      <c r="M459" s="1">
         <v>37.5</v>
       </c>
-      <c r="N459">
+      <c r="N459" s="1">
         <v>205</v>
       </c>
-      <c r="O459">
+      <c r="O459" s="1">
         <v>4.6402547039999999E-2</v>
       </c>
-    </row>
-    <row r="460" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P459" s="1">
+        <f t="shared" ref="P459:P465" si="4">(N459-N458)/(PI()*(M459^2-M458^2))</f>
+        <v>3.6261862234057439E-2</v>
+      </c>
+    </row>
+    <row r="460" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A460">
         <v>0.59</v>
       </c>
@@ -23115,7 +23135,7 @@
       <c r="I460">
         <v>25</v>
       </c>
-      <c r="J460">
+      <c r="J460" s="1">
         <v>0</v>
       </c>
       <c r="K460">
@@ -23124,17 +23144,21 @@
       <c r="L460">
         <v>25</v>
       </c>
-      <c r="M460">
+      <c r="M460" s="1">
         <v>50</v>
       </c>
-      <c r="N460">
+      <c r="N460" s="1">
         <v>330</v>
       </c>
-      <c r="O460">
+      <c r="O460" s="1">
         <v>4.2016940459999999E-2</v>
       </c>
-    </row>
-    <row r="461" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P460" s="1">
+        <f t="shared" si="4"/>
+        <v>3.6378272706718937E-2</v>
+      </c>
+    </row>
+    <row r="461" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A461">
         <v>0.59</v>
       </c>
@@ -23162,7 +23186,7 @@
       <c r="I461">
         <v>25</v>
       </c>
-      <c r="J461">
+      <c r="J461" s="1">
         <v>0</v>
       </c>
       <c r="K461">
@@ -23171,17 +23195,21 @@
       <c r="L461">
         <v>25</v>
       </c>
-      <c r="M461">
+      <c r="M461" s="1">
         <v>62.5</v>
       </c>
-      <c r="N461">
+      <c r="N461" s="1">
         <v>360</v>
       </c>
-      <c r="O461">
+      <c r="O461" s="1">
         <v>2.9335463879999999E-2</v>
       </c>
-    </row>
-    <row r="462" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P461" s="1">
+        <f t="shared" si="4"/>
+        <v>6.7906109052542005E-3</v>
+      </c>
+    </row>
+    <row r="462" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A462">
         <v>0.59</v>
       </c>
@@ -23209,7 +23237,7 @@
       <c r="I462">
         <v>25</v>
       </c>
-      <c r="J462">
+      <c r="J462" s="1">
         <v>0</v>
       </c>
       <c r="K462">
@@ -23218,17 +23246,21 @@
       <c r="L462">
         <v>25</v>
       </c>
-      <c r="M462">
-        <v>75</v>
-      </c>
-      <c r="N462">
+      <c r="M462" s="1">
+        <v>75</v>
+      </c>
+      <c r="N462" s="1">
         <v>366</v>
       </c>
-      <c r="O462">
+      <c r="O462" s="1">
         <v>2.0711380750000001E-2</v>
       </c>
-    </row>
-    <row r="463" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P462" s="1">
+        <f t="shared" si="4"/>
+        <v>1.1111908754052329E-3</v>
+      </c>
+    </row>
+    <row r="463" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A463">
         <v>0.59</v>
       </c>
@@ -23256,7 +23288,7 @@
       <c r="I463">
         <v>25</v>
       </c>
-      <c r="J463">
+      <c r="J463" s="1">
         <v>0</v>
       </c>
       <c r="K463">
@@ -23265,17 +23297,21 @@
       <c r="L463">
         <v>25</v>
       </c>
-      <c r="M463">
+      <c r="M463" s="1">
         <v>87.5</v>
       </c>
-      <c r="N463">
+      <c r="N463" s="1">
         <v>366</v>
       </c>
-      <c r="O463">
+      <c r="O463" s="1">
         <v>1.521652463E-2</v>
       </c>
-    </row>
-    <row r="464" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P463" s="1">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="464" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A464">
         <v>0.59</v>
       </c>
@@ -23303,7 +23339,7 @@
       <c r="I464">
         <v>25</v>
       </c>
-      <c r="J464">
+      <c r="J464" s="1">
         <v>0</v>
       </c>
       <c r="K464">
@@ -23312,17 +23348,21 @@
       <c r="L464">
         <v>25</v>
       </c>
-      <c r="M464">
+      <c r="M464" s="1">
         <v>100</v>
       </c>
-      <c r="N464">
+      <c r="N464" s="1">
         <v>366</v>
       </c>
-      <c r="O464">
+      <c r="O464" s="1">
         <v>1.1650151669999999E-2</v>
       </c>
-    </row>
-    <row r="465" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P464" s="1">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="465" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A465">
         <v>0.59</v>
       </c>
@@ -23350,7 +23390,7 @@
       <c r="I465">
         <v>25</v>
       </c>
-      <c r="J465">
+      <c r="J465" s="1">
         <v>0</v>
       </c>
       <c r="K465">
@@ -23359,17 +23399,21 @@
       <c r="L465">
         <v>25</v>
       </c>
-      <c r="M465">
+      <c r="M465" s="1">
         <v>112.5</v>
       </c>
-      <c r="N465">
+      <c r="N465" s="1">
         <v>368</v>
       </c>
-      <c r="O465">
+      <c r="O465" s="1">
         <v>9.2553589700000004E-3</v>
       </c>
-    </row>
-    <row r="466" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P465" s="1">
+        <f t="shared" si="4"/>
+        <v>2.396686201854424E-4</v>
+      </c>
+    </row>
+    <row r="466" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A466">
         <v>0.59</v>
       </c>
@@ -23397,26 +23441,30 @@
       <c r="I466">
         <v>25</v>
       </c>
-      <c r="J466">
-        <v>0</v>
+      <c r="J466" s="1">
+        <v>50</v>
       </c>
       <c r="K466">
         <v>2</v>
       </c>
       <c r="L466">
-        <v>25</v>
-      </c>
-      <c r="M466">
+        <v>75</v>
+      </c>
+      <c r="M466" s="1">
         <v>12.5</v>
       </c>
-      <c r="N466">
-        <v>27</v>
-      </c>
-      <c r="O466">
-        <v>5.5003994790000003E-2</v>
-      </c>
-    </row>
-    <row r="467" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="N466" s="1">
+        <v>4</v>
+      </c>
+      <c r="O466" s="1">
+        <v>8.14873996E-3</v>
+      </c>
+      <c r="P466" s="1">
+        <f>O466</f>
+        <v>8.14873996E-3</v>
+      </c>
+    </row>
+    <row r="467" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A467">
         <v>0.59</v>
       </c>
@@ -23444,7 +23492,7 @@
       <c r="I467">
         <v>25</v>
       </c>
-      <c r="J467">
+      <c r="J467" s="1">
         <v>50</v>
       </c>
       <c r="K467">
@@ -23453,17 +23501,21 @@
       <c r="L467">
         <v>75</v>
       </c>
-      <c r="M467">
-        <v>12.5</v>
-      </c>
-      <c r="N467">
-        <v>4</v>
-      </c>
-      <c r="O467">
-        <v>8.14873996E-3</v>
-      </c>
-    </row>
-    <row r="468" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="M467" s="1">
+        <v>25</v>
+      </c>
+      <c r="N467" s="1">
+        <v>28</v>
+      </c>
+      <c r="O467" s="1">
+        <v>1.4260294939999999E-2</v>
+      </c>
+      <c r="P467" s="1">
+        <f>(N467-N466)/(PI()*(M467^2-M466^2))</f>
+        <v>1.6297466172610083E-2</v>
+      </c>
+    </row>
+    <row r="468" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A468">
         <v>0.59</v>
       </c>
@@ -23491,7 +23543,7 @@
       <c r="I468">
         <v>25</v>
       </c>
-      <c r="J468">
+      <c r="J468" s="1">
         <v>50</v>
       </c>
       <c r="K468">
@@ -23500,17 +23552,21 @@
       <c r="L468">
         <v>75</v>
       </c>
-      <c r="M468">
-        <v>25</v>
-      </c>
-      <c r="N468">
-        <v>28</v>
-      </c>
-      <c r="O468">
-        <v>1.4260294939999999E-2</v>
-      </c>
-    </row>
-    <row r="469" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="M468" s="1">
+        <v>37.5</v>
+      </c>
+      <c r="N468" s="1">
+        <v>70</v>
+      </c>
+      <c r="O468" s="1">
+        <v>1.5844772159999999E-2</v>
+      </c>
+      <c r="P468" s="1">
+        <f t="shared" ref="P468:P474" si="5">(N468-N467)/(PI()*(M468^2-M467^2))</f>
+        <v>1.711233948124059E-2</v>
+      </c>
+    </row>
+    <row r="469" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A469">
         <v>0.59</v>
       </c>
@@ -23538,7 +23594,7 @@
       <c r="I469">
         <v>25</v>
       </c>
-      <c r="J469">
+      <c r="J469" s="1">
         <v>50</v>
       </c>
       <c r="K469">
@@ -23547,17 +23603,21 @@
       <c r="L469">
         <v>75</v>
       </c>
-      <c r="M469">
-        <v>37.5</v>
-      </c>
-      <c r="N469">
-        <v>70</v>
-      </c>
-      <c r="O469">
-        <v>1.5844772159999999E-2</v>
-      </c>
-    </row>
-    <row r="470" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="M469" s="1">
+        <v>50</v>
+      </c>
+      <c r="N469" s="1">
+        <v>100</v>
+      </c>
+      <c r="O469" s="1">
+        <v>1.2732406200000001E-2</v>
+      </c>
+      <c r="P469" s="1">
+        <f t="shared" si="5"/>
+        <v>8.7307854496125447E-3</v>
+      </c>
+    </row>
+    <row r="470" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A470">
         <v>0.59</v>
       </c>
@@ -23585,7 +23645,7 @@
       <c r="I470">
         <v>25</v>
       </c>
-      <c r="J470">
+      <c r="J470" s="1">
         <v>50</v>
       </c>
       <c r="K470">
@@ -23594,17 +23654,21 @@
       <c r="L470">
         <v>75</v>
       </c>
-      <c r="M470">
-        <v>50</v>
-      </c>
-      <c r="N470">
-        <v>100</v>
-      </c>
-      <c r="O470">
-        <v>1.2732406200000001E-2</v>
-      </c>
-    </row>
-    <row r="471" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="M470" s="1">
+        <v>62.5</v>
+      </c>
+      <c r="N470" s="1">
+        <v>157</v>
+      </c>
+      <c r="O470" s="1">
+        <v>1.279352175E-2</v>
+      </c>
+      <c r="P470" s="1">
+        <f t="shared" si="5"/>
+        <v>1.2902160719982982E-2</v>
+      </c>
+    </row>
+    <row r="471" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A471">
         <v>0.59</v>
       </c>
@@ -23632,7 +23696,7 @@
       <c r="I471">
         <v>25</v>
       </c>
-      <c r="J471">
+      <c r="J471" s="1">
         <v>50</v>
       </c>
       <c r="K471">
@@ -23641,17 +23705,21 @@
       <c r="L471">
         <v>75</v>
       </c>
-      <c r="M471">
-        <v>62.5</v>
-      </c>
-      <c r="N471">
-        <v>157</v>
-      </c>
-      <c r="O471">
-        <v>1.279352175E-2</v>
-      </c>
-    </row>
-    <row r="472" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="M471" s="1">
+        <v>75</v>
+      </c>
+      <c r="N471" s="1">
+        <v>210</v>
+      </c>
+      <c r="O471" s="1">
+        <v>1.188357912E-2</v>
+      </c>
+      <c r="P471" s="1">
+        <f t="shared" si="5"/>
+        <v>9.8155193994128916E-3</v>
+      </c>
+    </row>
+    <row r="472" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A472">
         <v>0.59</v>
       </c>
@@ -23679,7 +23747,7 @@
       <c r="I472">
         <v>25</v>
       </c>
-      <c r="J472">
+      <c r="J472" s="1">
         <v>50</v>
       </c>
       <c r="K472">
@@ -23688,17 +23756,21 @@
       <c r="L472">
         <v>75</v>
       </c>
-      <c r="M472">
-        <v>75</v>
-      </c>
-      <c r="N472">
-        <v>210</v>
-      </c>
-      <c r="O472">
-        <v>1.188357912E-2</v>
-      </c>
-    </row>
-    <row r="473" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="M472" s="1">
+        <v>87.5</v>
+      </c>
+      <c r="N472" s="1">
+        <v>288</v>
+      </c>
+      <c r="O472" s="1">
+        <v>1.197365873E-2</v>
+      </c>
+      <c r="P472" s="1">
+        <f t="shared" si="5"/>
+        <v>1.2223099629457562E-2</v>
+      </c>
+    </row>
+    <row r="473" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A473">
         <v>0.59</v>
       </c>
@@ -23726,7 +23798,7 @@
       <c r="I473">
         <v>25</v>
       </c>
-      <c r="J473">
+      <c r="J473" s="1">
         <v>50</v>
       </c>
       <c r="K473">
@@ -23735,17 +23807,21 @@
       <c r="L473">
         <v>75</v>
       </c>
-      <c r="M473">
-        <v>87.5</v>
-      </c>
-      <c r="N473">
-        <v>288</v>
-      </c>
-      <c r="O473">
-        <v>1.197365873E-2</v>
-      </c>
-    </row>
-    <row r="474" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="M473" s="1">
+        <v>100</v>
+      </c>
+      <c r="N473" s="1">
+        <v>349</v>
+      </c>
+      <c r="O473" s="1">
+        <v>1.110902441E-2</v>
+      </c>
+      <c r="P473" s="1">
+        <f t="shared" si="5"/>
+        <v>8.2845453044101264E-3</v>
+      </c>
+    </row>
+    <row r="474" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A474">
         <v>0.59</v>
       </c>
@@ -23773,7 +23849,7 @@
       <c r="I474">
         <v>25</v>
       </c>
-      <c r="J474">
+      <c r="J474" s="1">
         <v>50</v>
       </c>
       <c r="K474">
@@ -23782,17 +23858,21 @@
       <c r="L474">
         <v>75</v>
       </c>
-      <c r="M474">
-        <v>100</v>
-      </c>
-      <c r="N474">
-        <v>349</v>
-      </c>
-      <c r="O474">
-        <v>1.110902441E-2</v>
-      </c>
-    </row>
-    <row r="475" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="M474" s="1">
+        <v>112.5</v>
+      </c>
+      <c r="N474" s="1">
+        <v>363</v>
+      </c>
+      <c r="O474" s="1">
+        <v>9.1296068099999995E-3</v>
+      </c>
+      <c r="P474" s="1">
+        <f>(N474-N473)/(PI()*(M474^2-M473^2))</f>
+        <v>1.677680341298097E-3</v>
+      </c>
+    </row>
+    <row r="475" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A475">
         <v>0.59</v>
       </c>
@@ -23820,26 +23900,30 @@
       <c r="I475">
         <v>25</v>
       </c>
-      <c r="J475">
-        <v>50</v>
+      <c r="J475" s="1">
+        <v>100</v>
       </c>
       <c r="K475">
         <v>2</v>
       </c>
       <c r="L475">
-        <v>75</v>
-      </c>
-      <c r="M475">
-        <v>112.5</v>
-      </c>
-      <c r="N475">
-        <v>363</v>
-      </c>
-      <c r="O475">
-        <v>9.1296068099999995E-3</v>
-      </c>
-    </row>
-    <row r="476" spans="1:15" x14ac:dyDescent="0.3">
+        <v>125</v>
+      </c>
+      <c r="M475" s="1">
+        <v>12.5</v>
+      </c>
+      <c r="N475" s="1">
+        <v>0</v>
+      </c>
+      <c r="O475" s="1">
+        <v>0</v>
+      </c>
+      <c r="P475" s="1">
+        <f>O475</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="476" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A476">
         <v>0.59</v>
       </c>
@@ -23867,26 +23951,30 @@
       <c r="I476">
         <v>25</v>
       </c>
-      <c r="J476">
-        <v>50</v>
+      <c r="J476" s="1">
+        <v>100</v>
       </c>
       <c r="K476">
         <v>2</v>
       </c>
       <c r="L476">
-        <v>75</v>
-      </c>
-      <c r="M476">
-        <v>12.5</v>
-      </c>
-      <c r="N476">
+        <v>125</v>
+      </c>
+      <c r="M476" s="1">
+        <v>25</v>
+      </c>
+      <c r="N476" s="1">
         <v>4</v>
       </c>
-      <c r="O476">
-        <v>8.14873996E-3</v>
-      </c>
-    </row>
-    <row r="477" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="O476" s="1">
+        <v>2.03718499E-3</v>
+      </c>
+      <c r="P476" s="1">
+        <f>(N476-N475)/(PI()*(M476^2-M475^2))</f>
+        <v>2.7162443621016803E-3</v>
+      </c>
+    </row>
+    <row r="477" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A477">
         <v>0.59</v>
       </c>
@@ -23914,7 +24002,7 @@
       <c r="I477">
         <v>25</v>
       </c>
-      <c r="J477">
+      <c r="J477" s="1">
         <v>100</v>
       </c>
       <c r="K477">
@@ -23923,17 +24011,21 @@
       <c r="L477">
         <v>125</v>
       </c>
-      <c r="M477">
-        <v>12.5</v>
-      </c>
-      <c r="N477">
-        <v>0</v>
-      </c>
-      <c r="O477">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="478" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="M477" s="1">
+        <v>37.5</v>
+      </c>
+      <c r="N477" s="1">
+        <v>18</v>
+      </c>
+      <c r="O477" s="1">
+        <v>4.07436998E-3</v>
+      </c>
+      <c r="P477" s="1">
+        <f t="shared" ref="P477:P483" si="6">(N477-N476)/(PI()*(M477^2-M476^2))</f>
+        <v>5.7041131604135291E-3</v>
+      </c>
+    </row>
+    <row r="478" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A478">
         <v>0.59</v>
       </c>
@@ -23961,7 +24053,7 @@
       <c r="I478">
         <v>25</v>
       </c>
-      <c r="J478">
+      <c r="J478" s="1">
         <v>100</v>
       </c>
       <c r="K478">
@@ -23970,17 +24062,21 @@
       <c r="L478">
         <v>125</v>
       </c>
-      <c r="M478">
-        <v>25</v>
-      </c>
-      <c r="N478">
-        <v>4</v>
-      </c>
-      <c r="O478">
-        <v>2.03718499E-3</v>
-      </c>
-    </row>
-    <row r="479" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="M478" s="1">
+        <v>50</v>
+      </c>
+      <c r="N478" s="1">
+        <v>57</v>
+      </c>
+      <c r="O478" s="1">
+        <v>7.2574715300000002E-3</v>
+      </c>
+      <c r="P478" s="1">
+        <f t="shared" si="6"/>
+        <v>1.1350021084496308E-2</v>
+      </c>
+    </row>
+    <row r="479" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A479">
         <v>0.59</v>
       </c>
@@ -24008,7 +24104,7 @@
       <c r="I479">
         <v>25</v>
       </c>
-      <c r="J479">
+      <c r="J479" s="1">
         <v>100</v>
       </c>
       <c r="K479">
@@ -24017,17 +24113,21 @@
       <c r="L479">
         <v>125</v>
       </c>
-      <c r="M479">
-        <v>37.5</v>
-      </c>
-      <c r="N479">
-        <v>18</v>
-      </c>
-      <c r="O479">
-        <v>4.07436998E-3</v>
-      </c>
-    </row>
-    <row r="480" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="M479" s="1">
+        <v>62.5</v>
+      </c>
+      <c r="N479" s="1">
+        <v>79</v>
+      </c>
+      <c r="O479" s="1">
+        <v>6.4375045699999996E-3</v>
+      </c>
+      <c r="P479" s="1">
+        <f t="shared" si="6"/>
+        <v>4.979781330519747E-3</v>
+      </c>
+    </row>
+    <row r="480" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A480">
         <v>0.59</v>
       </c>
@@ -24055,7 +24155,7 @@
       <c r="I480">
         <v>25</v>
       </c>
-      <c r="J480">
+      <c r="J480" s="1">
         <v>100</v>
       </c>
       <c r="K480">
@@ -24064,17 +24164,21 @@
       <c r="L480">
         <v>125</v>
       </c>
-      <c r="M480">
-        <v>50</v>
-      </c>
-      <c r="N480">
-        <v>57</v>
-      </c>
-      <c r="O480">
-        <v>7.2574715300000002E-3</v>
-      </c>
-    </row>
-    <row r="481" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="M480" s="1">
+        <v>75</v>
+      </c>
+      <c r="N480" s="1">
+        <v>97</v>
+      </c>
+      <c r="O480" s="1">
+        <v>5.4890817800000002E-3</v>
+      </c>
+      <c r="P480" s="1">
+        <f t="shared" si="6"/>
+        <v>3.333572626215699E-3</v>
+      </c>
+    </row>
+    <row r="481" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A481">
         <v>0.59</v>
       </c>
@@ -24102,7 +24206,7 @@
       <c r="I481">
         <v>25</v>
       </c>
-      <c r="J481">
+      <c r="J481" s="1">
         <v>100</v>
       </c>
       <c r="K481">
@@ -24111,17 +24215,21 @@
       <c r="L481">
         <v>125</v>
       </c>
-      <c r="M481">
-        <v>62.5</v>
-      </c>
-      <c r="N481">
-        <v>79</v>
-      </c>
-      <c r="O481">
-        <v>6.4375045699999996E-3</v>
-      </c>
-    </row>
-    <row r="482" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="M481" s="1">
+        <v>87.5</v>
+      </c>
+      <c r="N481" s="1">
+        <v>135</v>
+      </c>
+      <c r="O481" s="1">
+        <v>5.6126525299999997E-3</v>
+      </c>
+      <c r="P481" s="1">
+        <f t="shared" si="6"/>
+        <v>5.9548434092229147E-3</v>
+      </c>
+    </row>
+    <row r="482" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A482">
         <v>0.59</v>
       </c>
@@ -24149,7 +24257,7 @@
       <c r="I482">
         <v>25</v>
       </c>
-      <c r="J482">
+      <c r="J482" s="1">
         <v>100</v>
       </c>
       <c r="K482">
@@ -24158,17 +24266,21 @@
       <c r="L482">
         <v>125</v>
       </c>
-      <c r="M482">
-        <v>75</v>
-      </c>
-      <c r="N482">
-        <v>97</v>
-      </c>
-      <c r="O482">
-        <v>5.4890817800000002E-3</v>
-      </c>
-    </row>
-    <row r="483" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="M482" s="1">
+        <v>100</v>
+      </c>
+      <c r="N482" s="1">
+        <v>183</v>
+      </c>
+      <c r="O482" s="1">
+        <v>5.82507583E-3</v>
+      </c>
+      <c r="P482" s="1">
+        <f t="shared" si="6"/>
+        <v>6.5189864690440328E-3</v>
+      </c>
+    </row>
+    <row r="483" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A483">
         <v>0.59</v>
       </c>
@@ -24196,7 +24308,7 @@
       <c r="I483">
         <v>25</v>
       </c>
-      <c r="J483">
+      <c r="J483" s="1">
         <v>100</v>
       </c>
       <c r="K483">
@@ -24205,17 +24317,21 @@
       <c r="L483">
         <v>125</v>
       </c>
-      <c r="M483">
-        <v>87.5</v>
-      </c>
-      <c r="N483">
-        <v>135</v>
-      </c>
-      <c r="O483">
-        <v>5.6126525299999997E-3</v>
-      </c>
-    </row>
-    <row r="484" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="M483" s="1">
+        <v>112.5</v>
+      </c>
+      <c r="N483" s="1">
+        <v>220</v>
+      </c>
+      <c r="O483" s="1">
+        <v>5.5330950399999999E-3</v>
+      </c>
+      <c r="P483" s="1">
+        <f t="shared" si="6"/>
+        <v>4.4338694734306844E-3</v>
+      </c>
+    </row>
+    <row r="484" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A484">
         <v>0.59</v>
       </c>
@@ -24243,26 +24359,30 @@
       <c r="I484">
         <v>25</v>
       </c>
-      <c r="J484">
-        <v>100</v>
+      <c r="J484" s="1">
+        <v>150</v>
       </c>
       <c r="K484">
         <v>2</v>
       </c>
       <c r="L484">
-        <v>125</v>
-      </c>
-      <c r="M484">
-        <v>100</v>
-      </c>
-      <c r="N484">
-        <v>183</v>
-      </c>
-      <c r="O484">
-        <v>5.82507583E-3</v>
-      </c>
-    </row>
-    <row r="485" spans="1:15" x14ac:dyDescent="0.3">
+        <v>175</v>
+      </c>
+      <c r="M484" s="1">
+        <v>12.5</v>
+      </c>
+      <c r="N484" s="1">
+        <v>0</v>
+      </c>
+      <c r="O484" s="1">
+        <v>0</v>
+      </c>
+      <c r="P484" s="1">
+        <f>O484</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="485" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A485">
         <v>0.59</v>
       </c>
@@ -24290,26 +24410,30 @@
       <c r="I485">
         <v>25</v>
       </c>
-      <c r="J485">
-        <v>100</v>
+      <c r="J485" s="1">
+        <v>150</v>
       </c>
       <c r="K485">
         <v>2</v>
       </c>
       <c r="L485">
-        <v>125</v>
-      </c>
-      <c r="M485">
-        <v>112.5</v>
-      </c>
-      <c r="N485">
-        <v>220</v>
-      </c>
-      <c r="O485">
-        <v>5.5330950399999999E-3</v>
-      </c>
-    </row>
-    <row r="486" spans="1:15" x14ac:dyDescent="0.3">
+        <v>175</v>
+      </c>
+      <c r="M485" s="1">
+        <v>25</v>
+      </c>
+      <c r="N485" s="1">
+        <v>0</v>
+      </c>
+      <c r="O485" s="1">
+        <v>0</v>
+      </c>
+      <c r="P485" s="1">
+        <f>(N485-N484)/(PI()*(M485^2-M484^2))</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="486" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A486">
         <v>0.59</v>
       </c>
@@ -24337,26 +24461,30 @@
       <c r="I486">
         <v>25</v>
       </c>
-      <c r="J486">
-        <v>100</v>
+      <c r="J486" s="1">
+        <v>150</v>
       </c>
       <c r="K486">
         <v>2</v>
       </c>
       <c r="L486">
-        <v>125</v>
-      </c>
-      <c r="M486">
-        <v>12.5</v>
-      </c>
-      <c r="N486">
-        <v>0</v>
-      </c>
-      <c r="O486">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="487" spans="1:15" x14ac:dyDescent="0.3">
+        <v>175</v>
+      </c>
+      <c r="M486" s="1">
+        <v>37.5</v>
+      </c>
+      <c r="N486" s="1">
+        <v>5</v>
+      </c>
+      <c r="O486" s="1">
+        <v>1.1317694399999999E-3</v>
+      </c>
+      <c r="P486" s="1">
+        <f t="shared" ref="P486:P492" si="7">(N486-N485)/(PI()*(M486^2-M485^2))</f>
+        <v>2.0371832715762603E-3</v>
+      </c>
+    </row>
+    <row r="487" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A487">
         <v>0.59</v>
       </c>
@@ -24384,7 +24512,7 @@
       <c r="I487">
         <v>25</v>
       </c>
-      <c r="J487">
+      <c r="J487" s="1">
         <v>150</v>
       </c>
       <c r="K487">
@@ -24393,17 +24521,21 @@
       <c r="L487">
         <v>175</v>
       </c>
-      <c r="M487">
-        <v>12.5</v>
-      </c>
-      <c r="N487">
-        <v>0</v>
-      </c>
-      <c r="O487">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="488" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="M487" s="1">
+        <v>50</v>
+      </c>
+      <c r="N487" s="1">
+        <v>13</v>
+      </c>
+      <c r="O487" s="1">
+        <v>1.6552127999999999E-3</v>
+      </c>
+      <c r="P487" s="1">
+        <f t="shared" si="7"/>
+        <v>2.328209453230012E-3</v>
+      </c>
+    </row>
+    <row r="488" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A488">
         <v>0.59</v>
       </c>
@@ -24431,7 +24563,7 @@
       <c r="I488">
         <v>25</v>
       </c>
-      <c r="J488">
+      <c r="J488" s="1">
         <v>150</v>
       </c>
       <c r="K488">
@@ -24440,17 +24572,21 @@
       <c r="L488">
         <v>175</v>
       </c>
-      <c r="M488">
-        <v>25</v>
-      </c>
-      <c r="N488">
-        <v>0</v>
-      </c>
-      <c r="O488">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="489" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="M488" s="1">
+        <v>62.5</v>
+      </c>
+      <c r="N488" s="1">
+        <v>44</v>
+      </c>
+      <c r="O488" s="1">
+        <v>3.5854455799999999E-3</v>
+      </c>
+      <c r="P488" s="1">
+        <f t="shared" si="7"/>
+        <v>7.0169646020960073E-3</v>
+      </c>
+    </row>
+    <row r="489" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A489">
         <v>0.59</v>
       </c>
@@ -24478,7 +24614,7 @@
       <c r="I489">
         <v>25</v>
       </c>
-      <c r="J489">
+      <c r="J489" s="1">
         <v>150</v>
       </c>
       <c r="K489">
@@ -24487,17 +24623,21 @@
       <c r="L489">
         <v>175</v>
       </c>
-      <c r="M489">
-        <v>37.5</v>
-      </c>
-      <c r="N489">
-        <v>5</v>
-      </c>
-      <c r="O489">
-        <v>1.1317694399999999E-3</v>
-      </c>
-    </row>
-    <row r="490" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="M489" s="1">
+        <v>75</v>
+      </c>
+      <c r="N489" s="1">
+        <v>58</v>
+      </c>
+      <c r="O489" s="1">
+        <v>3.28213137E-3</v>
+      </c>
+      <c r="P489" s="1">
+        <f t="shared" si="7"/>
+        <v>2.592778709278877E-3</v>
+      </c>
+    </row>
+    <row r="490" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A490">
         <v>0.59</v>
       </c>
@@ -24525,7 +24665,7 @@
       <c r="I490">
         <v>25</v>
       </c>
-      <c r="J490">
+      <c r="J490" s="1">
         <v>150</v>
       </c>
       <c r="K490">
@@ -24534,17 +24674,21 @@
       <c r="L490">
         <v>175</v>
       </c>
-      <c r="M490">
-        <v>50</v>
-      </c>
-      <c r="N490">
-        <v>13</v>
-      </c>
-      <c r="O490">
-        <v>1.6552127999999999E-3</v>
-      </c>
-    </row>
-    <row r="491" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="M490" s="1">
+        <v>87.5</v>
+      </c>
+      <c r="N490" s="1">
+        <v>81</v>
+      </c>
+      <c r="O490" s="1">
+        <v>3.3675915100000002E-3</v>
+      </c>
+      <c r="P490" s="1">
+        <f t="shared" si="7"/>
+        <v>3.6042473266349219E-3</v>
+      </c>
+    </row>
+    <row r="491" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A491">
         <v>0.59</v>
       </c>
@@ -24572,7 +24716,7 @@
       <c r="I491">
         <v>25</v>
       </c>
-      <c r="J491">
+      <c r="J491" s="1">
         <v>150</v>
       </c>
       <c r="K491">
@@ -24581,17 +24725,21 @@
       <c r="L491">
         <v>175</v>
       </c>
-      <c r="M491">
-        <v>62.5</v>
-      </c>
-      <c r="N491">
-        <v>44</v>
-      </c>
-      <c r="O491">
-        <v>3.5854455799999999E-3</v>
-      </c>
-    </row>
-    <row r="492" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="M491" s="1">
+        <v>100</v>
+      </c>
+      <c r="N491" s="1">
+        <v>99</v>
+      </c>
+      <c r="O491" s="1">
+        <v>3.1512705299999999E-3</v>
+      </c>
+      <c r="P491" s="1">
+        <f t="shared" si="7"/>
+        <v>2.4446199258915126E-3</v>
+      </c>
+    </row>
+    <row r="492" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A492">
         <v>0.59</v>
       </c>
@@ -24619,7 +24767,7 @@
       <c r="I492">
         <v>25</v>
       </c>
-      <c r="J492">
+      <c r="J492" s="1">
         <v>150</v>
       </c>
       <c r="K492">
@@ -24628,116 +24776,81 @@
       <c r="L492">
         <v>175</v>
       </c>
-      <c r="M492">
-        <v>75</v>
-      </c>
-      <c r="N492">
-        <v>58</v>
-      </c>
-      <c r="O492">
-        <v>3.28213137E-3</v>
-      </c>
-    </row>
-    <row r="493" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A493">
-        <v>0.59</v>
-      </c>
-      <c r="B493">
-        <v>1.768</v>
-      </c>
-      <c r="C493">
-        <v>-1</v>
-      </c>
-      <c r="D493">
-        <v>25</v>
-      </c>
-      <c r="E493">
-        <v>32.692</v>
-      </c>
-      <c r="F493">
-        <v>20.192</v>
-      </c>
-      <c r="G493">
-        <v>25</v>
-      </c>
-      <c r="H493">
-        <v>12.5</v>
-      </c>
-      <c r="I493">
-        <v>25</v>
-      </c>
-      <c r="J493">
-        <v>150</v>
-      </c>
-      <c r="K493">
-        <v>2</v>
-      </c>
-      <c r="L493">
-        <v>175</v>
-      </c>
-      <c r="M493">
-        <v>87.5</v>
-      </c>
-      <c r="N493">
-        <v>81</v>
-      </c>
-      <c r="O493">
-        <v>3.3675915100000002E-3</v>
-      </c>
-    </row>
-    <row r="494" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A494">
-        <v>0.59</v>
-      </c>
-      <c r="B494">
-        <v>1.768</v>
-      </c>
-      <c r="C494">
-        <v>-1</v>
-      </c>
-      <c r="D494">
-        <v>25</v>
-      </c>
-      <c r="E494">
-        <v>32.692</v>
-      </c>
-      <c r="F494">
-        <v>20.192</v>
-      </c>
-      <c r="G494">
-        <v>25</v>
-      </c>
-      <c r="H494">
-        <v>12.5</v>
-      </c>
-      <c r="I494">
-        <v>25</v>
-      </c>
-      <c r="J494">
-        <v>150</v>
-      </c>
-      <c r="K494">
-        <v>2</v>
-      </c>
-      <c r="L494">
-        <v>175</v>
-      </c>
-      <c r="M494">
-        <v>100</v>
-      </c>
-      <c r="N494">
-        <v>99</v>
-      </c>
-      <c r="O494">
-        <v>3.1512705299999999E-3</v>
-      </c>
-    </row>
-    <row r="495" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="M492" s="1">
+        <v>112.5</v>
+      </c>
+      <c r="N492" s="1">
+        <v>123</v>
+      </c>
+      <c r="O492" s="1">
+        <v>3.09350313E-3</v>
+      </c>
+      <c r="P492" s="1">
+        <f t="shared" si="7"/>
+        <v>2.876023442225309E-3</v>
+      </c>
+    </row>
+    <row r="493" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A493" t="s">
+        <v>22</v>
+      </c>
+      <c r="B493" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="494" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A494" t="s">
+        <v>1</v>
+      </c>
+      <c r="B494" t="s">
+        <v>2</v>
+      </c>
+      <c r="C494" t="s">
+        <v>19</v>
+      </c>
+      <c r="D494" t="s">
+        <v>3</v>
+      </c>
+      <c r="E494" t="s">
+        <v>4</v>
+      </c>
+      <c r="F494" t="s">
+        <v>5</v>
+      </c>
+      <c r="G494" t="s">
+        <v>6</v>
+      </c>
+      <c r="H494" t="s">
+        <v>7</v>
+      </c>
+      <c r="I494" t="s">
+        <v>8</v>
+      </c>
+      <c r="J494" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="K494" t="s">
+        <v>10</v>
+      </c>
+      <c r="L494" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="M494" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="N494" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="O494" s="4" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="495" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A495">
         <v>0.59</v>
       </c>
       <c r="B495">
-        <v>1.768</v>
+        <v>2.1</v>
       </c>
       <c r="C495">
         <v>-1</v>
@@ -24746,10 +24859,10 @@
         <v>25</v>
       </c>
       <c r="E495">
-        <v>32.692</v>
+        <v>19.588999999999999</v>
       </c>
       <c r="F495">
-        <v>20.192</v>
+        <v>7.0895000000000001</v>
       </c>
       <c r="G495">
         <v>25</v>
@@ -24761,30 +24874,30 @@
         <v>25</v>
       </c>
       <c r="J495">
-        <v>150</v>
+        <v>0</v>
       </c>
       <c r="K495">
         <v>2</v>
       </c>
       <c r="L495">
-        <v>175</v>
+        <v>25</v>
       </c>
       <c r="M495">
-        <v>112.5</v>
+        <v>12.5</v>
       </c>
       <c r="N495">
-        <v>123</v>
+        <v>28</v>
       </c>
       <c r="O495">
-        <v>3.09350313E-3</v>
-      </c>
-    </row>
-    <row r="496" spans="1:15" x14ac:dyDescent="0.3">
+        <v>5.7041179779999999E-2</v>
+      </c>
+    </row>
+    <row r="496" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A496">
         <v>0.59</v>
       </c>
       <c r="B496">
-        <v>1.768</v>
+        <v>2.1</v>
       </c>
       <c r="C496">
         <v>-1</v>
@@ -24793,10 +24906,10 @@
         <v>25</v>
       </c>
       <c r="E496">
-        <v>32.692</v>
+        <v>19.588999999999999</v>
       </c>
       <c r="F496">
-        <v>20.192</v>
+        <v>7.0895000000000001</v>
       </c>
       <c r="G496">
         <v>25</v>
@@ -24808,77 +24921,116 @@
         <v>25</v>
       </c>
       <c r="J496">
-        <v>150</v>
+        <v>0</v>
       </c>
       <c r="K496">
         <v>2</v>
       </c>
       <c r="L496">
-        <v>175</v>
+        <v>25</v>
       </c>
       <c r="M496">
+        <v>25</v>
+      </c>
+      <c r="N496">
+        <v>116</v>
+      </c>
+      <c r="O496">
+        <v>5.9078364770000003E-2</v>
+      </c>
+    </row>
+    <row r="497" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A497">
+        <v>0.59</v>
+      </c>
+      <c r="B497">
+        <v>2.1</v>
+      </c>
+      <c r="C497">
+        <v>-1</v>
+      </c>
+      <c r="D497">
+        <v>25</v>
+      </c>
+      <c r="E497">
+        <v>19.588999999999999</v>
+      </c>
+      <c r="F497">
+        <v>7.0895000000000001</v>
+      </c>
+      <c r="G497">
+        <v>25</v>
+      </c>
+      <c r="H497">
         <v>12.5</v>
       </c>
-      <c r="N496">
+      <c r="I497">
+        <v>25</v>
+      </c>
+      <c r="J497">
         <v>0</v>
       </c>
-      <c r="O496">
+      <c r="K497">
+        <v>2</v>
+      </c>
+      <c r="L497">
+        <v>25</v>
+      </c>
+      <c r="M497">
+        <v>37.5</v>
+      </c>
+      <c r="N497">
+        <v>206</v>
+      </c>
+      <c r="O497">
+        <v>4.6628900930000002E-2</v>
+      </c>
+    </row>
+    <row r="498" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A498">
+        <v>0.59</v>
+      </c>
+      <c r="B498">
+        <v>2.1</v>
+      </c>
+      <c r="C498">
+        <v>-1</v>
+      </c>
+      <c r="D498">
+        <v>25</v>
+      </c>
+      <c r="E498">
+        <v>19.588999999999999</v>
+      </c>
+      <c r="F498">
+        <v>7.0895000000000001</v>
+      </c>
+      <c r="G498">
+        <v>25</v>
+      </c>
+      <c r="H498">
+        <v>12.5</v>
+      </c>
+      <c r="I498">
+        <v>25</v>
+      </c>
+      <c r="J498">
         <v>0</v>
       </c>
-    </row>
-    <row r="497" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A497" t="s">
-        <v>22</v>
-      </c>
-      <c r="B497" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="498" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A498" t="s">
-        <v>1</v>
-      </c>
-      <c r="B498" t="s">
-        <v>2</v>
-      </c>
-      <c r="C498" t="s">
-        <v>19</v>
-      </c>
-      <c r="D498" t="s">
-        <v>3</v>
-      </c>
-      <c r="E498" t="s">
-        <v>4</v>
-      </c>
-      <c r="F498" t="s">
-        <v>5</v>
-      </c>
-      <c r="G498" t="s">
-        <v>6</v>
-      </c>
-      <c r="H498" t="s">
-        <v>7</v>
-      </c>
-      <c r="I498" t="s">
-        <v>8</v>
-      </c>
-      <c r="J498" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="K498" t="s">
-        <v>10</v>
-      </c>
-      <c r="L498" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="M498" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="N498" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="O498" s="4" t="s">
-        <v>14</v>
+      <c r="K498">
+        <v>2</v>
+      </c>
+      <c r="L498">
+        <v>25</v>
+      </c>
+      <c r="M498">
+        <v>50</v>
+      </c>
+      <c r="N498">
+        <v>332</v>
+      </c>
+      <c r="O498">
+        <v>4.2271588589999999E-2</v>
       </c>
     </row>
     <row r="499" spans="1:15" x14ac:dyDescent="0.3">
@@ -24919,13 +25071,13 @@
         <v>25</v>
       </c>
       <c r="M499">
-        <v>12.5</v>
+        <v>62.5</v>
       </c>
       <c r="N499">
-        <v>28</v>
+        <v>362</v>
       </c>
       <c r="O499">
-        <v>5.7041179779999999E-2</v>
+        <v>2.9498438679999999E-2</v>
       </c>
     </row>
     <row r="500" spans="1:15" x14ac:dyDescent="0.3">
@@ -24966,13 +25118,13 @@
         <v>25</v>
       </c>
       <c r="M500">
-        <v>25</v>
+        <v>75</v>
       </c>
       <c r="N500">
-        <v>116</v>
+        <v>364</v>
       </c>
       <c r="O500">
-        <v>5.9078364770000003E-2</v>
+        <v>2.059820381E-2</v>
       </c>
     </row>
     <row r="501" spans="1:15" x14ac:dyDescent="0.3">
@@ -25013,13 +25165,13 @@
         <v>25</v>
       </c>
       <c r="M501">
-        <v>37.5</v>
+        <v>87.5</v>
       </c>
       <c r="N501">
-        <v>206</v>
+        <v>366</v>
       </c>
       <c r="O501">
-        <v>4.6628900930000002E-2</v>
+        <v>1.521652463E-2</v>
       </c>
     </row>
     <row r="502" spans="1:15" x14ac:dyDescent="0.3">
@@ -25060,13 +25212,13 @@
         <v>25</v>
       </c>
       <c r="M502">
-        <v>50</v>
+        <v>100</v>
       </c>
       <c r="N502">
-        <v>332</v>
+        <v>366</v>
       </c>
       <c r="O502">
-        <v>4.2271588589999999E-2</v>
+        <v>1.1650151669999999E-2</v>
       </c>
     </row>
     <row r="503" spans="1:15" x14ac:dyDescent="0.3">
@@ -25107,13 +25259,13 @@
         <v>25</v>
       </c>
       <c r="M503">
-        <v>62.5</v>
+        <v>112.5</v>
       </c>
       <c r="N503">
-        <v>362</v>
+        <v>369</v>
       </c>
       <c r="O503">
-        <v>2.9498438679999999E-2</v>
+        <v>9.2805093999999994E-3</v>
       </c>
     </row>
     <row r="504" spans="1:15" x14ac:dyDescent="0.3">
@@ -25154,13 +25306,13 @@
         <v>25</v>
       </c>
       <c r="M504">
-        <v>75</v>
+        <v>12.5</v>
       </c>
       <c r="N504">
-        <v>364</v>
+        <v>28</v>
       </c>
       <c r="O504">
-        <v>2.059820381E-2</v>
+        <v>5.7041179779999999E-2</v>
       </c>
     </row>
     <row r="505" spans="1:15" x14ac:dyDescent="0.3">
@@ -25192,22 +25344,22 @@
         <v>25</v>
       </c>
       <c r="J505">
-        <v>0</v>
+        <v>50</v>
       </c>
       <c r="K505">
         <v>2</v>
       </c>
       <c r="L505">
-        <v>25</v>
+        <v>75</v>
       </c>
       <c r="M505">
-        <v>87.5</v>
+        <v>12.5</v>
       </c>
       <c r="N505">
-        <v>366</v>
+        <v>3</v>
       </c>
       <c r="O505">
-        <v>1.521652463E-2</v>
+        <v>6.1115549700000004E-3</v>
       </c>
     </row>
     <row r="506" spans="1:15" x14ac:dyDescent="0.3">
@@ -25239,22 +25391,22 @@
         <v>25</v>
       </c>
       <c r="J506">
-        <v>0</v>
+        <v>50</v>
       </c>
       <c r="K506">
         <v>2</v>
       </c>
       <c r="L506">
-        <v>25</v>
+        <v>75</v>
       </c>
       <c r="M506">
-        <v>100</v>
+        <v>25</v>
       </c>
       <c r="N506">
-        <v>366</v>
+        <v>31</v>
       </c>
       <c r="O506">
-        <v>1.1650151669999999E-2</v>
+        <v>1.5788183689999999E-2</v>
       </c>
     </row>
     <row r="507" spans="1:15" x14ac:dyDescent="0.3">
@@ -25286,22 +25438,22 @@
         <v>25</v>
       </c>
       <c r="J507">
-        <v>0</v>
+        <v>50</v>
       </c>
       <c r="K507">
         <v>2</v>
       </c>
       <c r="L507">
-        <v>25</v>
+        <v>75</v>
       </c>
       <c r="M507">
-        <v>112.5</v>
+        <v>37.5</v>
       </c>
       <c r="N507">
-        <v>369</v>
+        <v>67</v>
       </c>
       <c r="O507">
-        <v>9.2805093999999994E-3</v>
+        <v>1.516571049E-2</v>
       </c>
     </row>
     <row r="508" spans="1:15" x14ac:dyDescent="0.3">
@@ -25333,22 +25485,22 @@
         <v>25</v>
       </c>
       <c r="J508">
-        <v>0</v>
+        <v>50</v>
       </c>
       <c r="K508">
         <v>2</v>
       </c>
       <c r="L508">
-        <v>25</v>
+        <v>75</v>
       </c>
       <c r="M508">
-        <v>12.5</v>
+        <v>50</v>
       </c>
       <c r="N508">
-        <v>28</v>
+        <v>98</v>
       </c>
       <c r="O508">
-        <v>5.7041179779999999E-2</v>
+        <v>1.2477758070000001E-2</v>
       </c>
     </row>
     <row r="509" spans="1:15" x14ac:dyDescent="0.3">
@@ -25389,13 +25541,13 @@
         <v>75</v>
       </c>
       <c r="M509">
-        <v>12.5</v>
+        <v>62.5</v>
       </c>
       <c r="N509">
-        <v>3</v>
+        <v>153</v>
       </c>
       <c r="O509">
-        <v>6.1115549700000004E-3</v>
+        <v>1.246757215E-2</v>
       </c>
     </row>
     <row r="510" spans="1:15" x14ac:dyDescent="0.3">
@@ -25436,13 +25588,13 @@
         <v>75</v>
       </c>
       <c r="M510">
-        <v>25</v>
+        <v>75</v>
       </c>
       <c r="N510">
-        <v>31</v>
+        <v>214</v>
       </c>
       <c r="O510">
-        <v>1.5788183689999999E-2</v>
+        <v>1.2109933010000001E-2</v>
       </c>
     </row>
     <row r="511" spans="1:15" x14ac:dyDescent="0.3">
@@ -25483,13 +25635,13 @@
         <v>75</v>
       </c>
       <c r="M511">
-        <v>37.5</v>
+        <v>87.5</v>
       </c>
       <c r="N511">
-        <v>67</v>
+        <v>288</v>
       </c>
       <c r="O511">
-        <v>1.516571049E-2</v>
+        <v>1.197365873E-2</v>
       </c>
     </row>
     <row r="512" spans="1:15" x14ac:dyDescent="0.3">
@@ -25530,13 +25682,13 @@
         <v>75</v>
       </c>
       <c r="M512">
-        <v>50</v>
+        <v>100</v>
       </c>
       <c r="N512">
-        <v>98</v>
+        <v>345</v>
       </c>
       <c r="O512">
-        <v>1.2477758070000001E-2</v>
+        <v>1.0981700340000001E-2</v>
       </c>
     </row>
     <row r="513" spans="1:15" x14ac:dyDescent="0.3">
@@ -25577,13 +25729,13 @@
         <v>75</v>
       </c>
       <c r="M513">
-        <v>62.5</v>
+        <v>112.5</v>
       </c>
       <c r="N513">
-        <v>153</v>
+        <v>361</v>
       </c>
       <c r="O513">
-        <v>1.246757215E-2</v>
+        <v>9.0793059499999999E-3</v>
       </c>
     </row>
     <row r="514" spans="1:15" x14ac:dyDescent="0.3">
@@ -25624,13 +25776,13 @@
         <v>75</v>
       </c>
       <c r="M514">
-        <v>75</v>
+        <v>12.5</v>
       </c>
       <c r="N514">
-        <v>214</v>
+        <v>3</v>
       </c>
       <c r="O514">
-        <v>1.2109933010000001E-2</v>
+        <v>6.1115549700000004E-3</v>
       </c>
     </row>
     <row r="515" spans="1:15" x14ac:dyDescent="0.3">
@@ -25662,22 +25814,22 @@
         <v>25</v>
       </c>
       <c r="J515">
-        <v>50</v>
+        <v>100</v>
       </c>
       <c r="K515">
         <v>2</v>
       </c>
       <c r="L515">
-        <v>75</v>
+        <v>125</v>
       </c>
       <c r="M515">
-        <v>87.5</v>
+        <v>12.5</v>
       </c>
       <c r="N515">
-        <v>288</v>
+        <v>1</v>
       </c>
       <c r="O515">
-        <v>1.197365873E-2</v>
+        <v>2.03718499E-3</v>
       </c>
     </row>
     <row r="516" spans="1:15" x14ac:dyDescent="0.3">
@@ -25709,22 +25861,22 @@
         <v>25</v>
       </c>
       <c r="J516">
-        <v>50</v>
+        <v>100</v>
       </c>
       <c r="K516">
         <v>2</v>
       </c>
       <c r="L516">
-        <v>75</v>
+        <v>125</v>
       </c>
       <c r="M516">
-        <v>100</v>
+        <v>25</v>
       </c>
       <c r="N516">
-        <v>345</v>
+        <v>3</v>
       </c>
       <c r="O516">
-        <v>1.0981700340000001E-2</v>
+        <v>1.5278887399999999E-3</v>
       </c>
     </row>
     <row r="517" spans="1:15" x14ac:dyDescent="0.3">
@@ -25756,22 +25908,22 @@
         <v>25</v>
       </c>
       <c r="J517">
-        <v>50</v>
+        <v>100</v>
       </c>
       <c r="K517">
         <v>2</v>
       </c>
       <c r="L517">
-        <v>75</v>
+        <v>125</v>
       </c>
       <c r="M517">
-        <v>112.5</v>
+        <v>37.5</v>
       </c>
       <c r="N517">
-        <v>361</v>
+        <v>16</v>
       </c>
       <c r="O517">
-        <v>9.0793059499999999E-3</v>
+        <v>3.6216622E-3</v>
       </c>
     </row>
     <row r="518" spans="1:15" x14ac:dyDescent="0.3">
@@ -25803,22 +25955,22 @@
         <v>25</v>
       </c>
       <c r="J518">
+        <v>100</v>
+      </c>
+      <c r="K518">
+        <v>2</v>
+      </c>
+      <c r="L518">
+        <v>125</v>
+      </c>
+      <c r="M518">
         <v>50</v>
       </c>
-      <c r="K518">
-        <v>2</v>
-      </c>
-      <c r="L518">
-        <v>75</v>
-      </c>
-      <c r="M518">
-        <v>12.5</v>
-      </c>
       <c r="N518">
-        <v>3</v>
+        <v>54</v>
       </c>
       <c r="O518">
-        <v>6.1115549700000004E-3</v>
+        <v>6.8754993399999997E-3</v>
       </c>
     </row>
     <row r="519" spans="1:15" x14ac:dyDescent="0.3">
@@ -25859,13 +26011,13 @@
         <v>125</v>
       </c>
       <c r="M519">
-        <v>12.5</v>
+        <v>62.5</v>
       </c>
       <c r="N519">
-        <v>1</v>
+        <v>81</v>
       </c>
       <c r="O519">
-        <v>2.03718499E-3</v>
+        <v>6.6004793699999996E-3</v>
       </c>
     </row>
     <row r="520" spans="1:15" x14ac:dyDescent="0.3">
@@ -25906,13 +26058,13 @@
         <v>125</v>
       </c>
       <c r="M520">
-        <v>25</v>
+        <v>75</v>
       </c>
       <c r="N520">
-        <v>3</v>
+        <v>104</v>
       </c>
       <c r="O520">
-        <v>1.5278887399999999E-3</v>
+        <v>5.8852010800000002E-3</v>
       </c>
     </row>
     <row r="521" spans="1:15" x14ac:dyDescent="0.3">
@@ -25953,13 +26105,13 @@
         <v>125</v>
       </c>
       <c r="M521">
-        <v>37.5</v>
+        <v>87.5</v>
       </c>
       <c r="N521">
-        <v>16</v>
+        <v>142</v>
       </c>
       <c r="O521">
-        <v>3.6216622E-3</v>
+        <v>5.9036789500000004E-3</v>
       </c>
     </row>
     <row r="522" spans="1:15" x14ac:dyDescent="0.3">
@@ -26000,13 +26152,13 @@
         <v>125</v>
       </c>
       <c r="M522">
-        <v>50</v>
+        <v>100</v>
       </c>
       <c r="N522">
-        <v>54</v>
+        <v>191</v>
       </c>
       <c r="O522">
-        <v>6.8754993399999997E-3</v>
+        <v>6.0797239600000001E-3</v>
       </c>
     </row>
     <row r="523" spans="1:15" x14ac:dyDescent="0.3">
@@ -26047,13 +26199,13 @@
         <v>125</v>
       </c>
       <c r="M523">
-        <v>62.5</v>
+        <v>112.5</v>
       </c>
       <c r="N523">
-        <v>81</v>
+        <v>230</v>
       </c>
       <c r="O523">
-        <v>6.6004793699999996E-3</v>
+        <v>5.7845993599999999E-3</v>
       </c>
     </row>
     <row r="524" spans="1:15" x14ac:dyDescent="0.3">
@@ -26094,13 +26246,13 @@
         <v>125</v>
       </c>
       <c r="M524">
-        <v>75</v>
+        <v>12.5</v>
       </c>
       <c r="N524">
-        <v>104</v>
+        <v>1</v>
       </c>
       <c r="O524">
-        <v>5.8852010800000002E-3</v>
+        <v>2.03718499E-3</v>
       </c>
     </row>
     <row r="525" spans="1:15" x14ac:dyDescent="0.3">
@@ -26132,22 +26284,22 @@
         <v>25</v>
       </c>
       <c r="J525">
-        <v>100</v>
+        <v>150</v>
       </c>
       <c r="K525">
         <v>2</v>
       </c>
       <c r="L525">
-        <v>125</v>
+        <v>175</v>
       </c>
       <c r="M525">
-        <v>87.5</v>
+        <v>12.5</v>
       </c>
       <c r="N525">
-        <v>142</v>
+        <v>0</v>
       </c>
       <c r="O525">
-        <v>5.9036789500000004E-3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="526" spans="1:15" x14ac:dyDescent="0.3">
@@ -26179,22 +26331,22 @@
         <v>25</v>
       </c>
       <c r="J526">
-        <v>100</v>
+        <v>150</v>
       </c>
       <c r="K526">
         <v>2</v>
       </c>
       <c r="L526">
-        <v>125</v>
+        <v>175</v>
       </c>
       <c r="M526">
-        <v>100</v>
+        <v>25</v>
       </c>
       <c r="N526">
-        <v>191</v>
+        <v>1</v>
       </c>
       <c r="O526">
-        <v>6.0797239600000001E-3</v>
+        <v>5.0929624000000003E-4</v>
       </c>
     </row>
     <row r="527" spans="1:15" x14ac:dyDescent="0.3">
@@ -26226,22 +26378,22 @@
         <v>25</v>
       </c>
       <c r="J527">
-        <v>100</v>
+        <v>150</v>
       </c>
       <c r="K527">
         <v>2</v>
       </c>
       <c r="L527">
-        <v>125</v>
+        <v>175</v>
       </c>
       <c r="M527">
-        <v>112.5</v>
+        <v>37.5</v>
       </c>
       <c r="N527">
-        <v>230</v>
+        <v>4</v>
       </c>
       <c r="O527">
-        <v>5.7845993599999999E-3</v>
+        <v>9.0541554999999999E-4</v>
       </c>
     </row>
     <row r="528" spans="1:15" x14ac:dyDescent="0.3">
@@ -26273,22 +26425,22 @@
         <v>25</v>
       </c>
       <c r="J528">
-        <v>100</v>
+        <v>150</v>
       </c>
       <c r="K528">
         <v>2</v>
       </c>
       <c r="L528">
-        <v>125</v>
+        <v>175</v>
       </c>
       <c r="M528">
-        <v>12.5</v>
+        <v>50</v>
       </c>
       <c r="N528">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="O528">
-        <v>2.03718499E-3</v>
+        <v>1.5278887399999999E-3</v>
       </c>
     </row>
     <row r="529" spans="1:15" x14ac:dyDescent="0.3">
@@ -26329,13 +26481,13 @@
         <v>175</v>
       </c>
       <c r="M529">
-        <v>12.5</v>
+        <v>62.5</v>
       </c>
       <c r="N529">
-        <v>0</v>
+        <v>45</v>
       </c>
       <c r="O529">
-        <v>0</v>
+        <v>3.6669329799999999E-3</v>
       </c>
     </row>
     <row r="530" spans="1:15" x14ac:dyDescent="0.3">
@@ -26376,13 +26528,13 @@
         <v>175</v>
       </c>
       <c r="M530">
-        <v>25</v>
+        <v>75</v>
       </c>
       <c r="N530">
-        <v>1</v>
+        <v>59</v>
       </c>
       <c r="O530">
-        <v>5.0929624000000003E-4</v>
+        <v>3.3387198400000001E-3</v>
       </c>
     </row>
     <row r="531" spans="1:15" x14ac:dyDescent="0.3">
@@ -26423,13 +26575,13 @@
         <v>175</v>
       </c>
       <c r="M531">
-        <v>37.5</v>
+        <v>87.5</v>
       </c>
       <c r="N531">
-        <v>4</v>
+        <v>77</v>
       </c>
       <c r="O531">
-        <v>9.0541554999999999E-4</v>
+        <v>3.2012907000000001E-3</v>
       </c>
     </row>
     <row r="532" spans="1:15" x14ac:dyDescent="0.3">
@@ -26470,13 +26622,13 @@
         <v>175</v>
       </c>
       <c r="M532">
-        <v>50</v>
+        <v>100</v>
       </c>
       <c r="N532">
-        <v>12</v>
+        <v>96</v>
       </c>
       <c r="O532">
-        <v>1.5278887399999999E-3</v>
+        <v>3.0557774799999998E-3</v>
       </c>
     </row>
     <row r="533" spans="1:15" x14ac:dyDescent="0.3">
@@ -26517,13 +26669,13 @@
         <v>175</v>
       </c>
       <c r="M533">
-        <v>62.5</v>
+        <v>112.5</v>
       </c>
       <c r="N533">
-        <v>45</v>
+        <v>117</v>
       </c>
       <c r="O533">
-        <v>3.6669329799999999E-3</v>
+        <v>2.9426005400000001E-3</v>
       </c>
     </row>
     <row r="534" spans="1:15" x14ac:dyDescent="0.3">
@@ -26564,13 +26716,13 @@
         <v>175</v>
       </c>
       <c r="M534">
-        <v>75</v>
+        <v>12.5</v>
       </c>
       <c r="N534">
-        <v>59</v>
+        <v>0</v>
       </c>
       <c r="O534">
-        <v>3.3387198400000001E-3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="535" spans="1:15" x14ac:dyDescent="0.3">
@@ -26602,22 +26754,22 @@
         <v>25</v>
       </c>
       <c r="J535">
-        <v>150</v>
+        <v>0</v>
       </c>
       <c r="K535">
         <v>2</v>
       </c>
       <c r="L535">
-        <v>175</v>
+        <v>25</v>
       </c>
       <c r="M535">
-        <v>87.5</v>
+        <v>12.5</v>
       </c>
       <c r="N535">
-        <v>77</v>
+        <v>28</v>
       </c>
       <c r="O535">
-        <v>3.2012907000000001E-3</v>
+        <v>5.7041179779999999E-2</v>
       </c>
     </row>
     <row r="536" spans="1:15" x14ac:dyDescent="0.3">
@@ -26649,22 +26801,22 @@
         <v>25</v>
       </c>
       <c r="J536">
-        <v>150</v>
+        <v>0</v>
       </c>
       <c r="K536">
         <v>2</v>
       </c>
       <c r="L536">
-        <v>175</v>
+        <v>25</v>
       </c>
       <c r="M536">
-        <v>100</v>
+        <v>25</v>
       </c>
       <c r="N536">
-        <v>96</v>
+        <v>116</v>
       </c>
       <c r="O536">
-        <v>3.0557774799999998E-3</v>
+        <v>5.9078364770000003E-2</v>
       </c>
     </row>
     <row r="537" spans="1:15" x14ac:dyDescent="0.3">
@@ -26696,209 +26848,21 @@
         <v>25</v>
       </c>
       <c r="J537">
-        <v>150</v>
+        <v>0</v>
       </c>
       <c r="K537">
         <v>2</v>
       </c>
       <c r="L537">
-        <v>175</v>
+        <v>25</v>
       </c>
       <c r="M537">
-        <v>112.5</v>
+        <v>37.5</v>
       </c>
       <c r="N537">
-        <v>117</v>
+        <v>206</v>
       </c>
       <c r="O537">
-        <v>2.9426005400000001E-3</v>
-      </c>
-    </row>
-    <row r="538" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A538">
-        <v>0.59</v>
-      </c>
-      <c r="B538">
-        <v>2.1</v>
-      </c>
-      <c r="C538">
-        <v>-1</v>
-      </c>
-      <c r="D538">
-        <v>25</v>
-      </c>
-      <c r="E538">
-        <v>19.588999999999999</v>
-      </c>
-      <c r="F538">
-        <v>7.0895000000000001</v>
-      </c>
-      <c r="G538">
-        <v>25</v>
-      </c>
-      <c r="H538">
-        <v>12.5</v>
-      </c>
-      <c r="I538">
-        <v>25</v>
-      </c>
-      <c r="J538">
-        <v>150</v>
-      </c>
-      <c r="K538">
-        <v>2</v>
-      </c>
-      <c r="L538">
-        <v>175</v>
-      </c>
-      <c r="M538">
-        <v>12.5</v>
-      </c>
-      <c r="N538">
-        <v>0</v>
-      </c>
-      <c r="O538">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="539" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A539">
-        <v>0.59</v>
-      </c>
-      <c r="B539">
-        <v>2.1</v>
-      </c>
-      <c r="C539">
-        <v>-1</v>
-      </c>
-      <c r="D539">
-        <v>25</v>
-      </c>
-      <c r="E539">
-        <v>19.588999999999999</v>
-      </c>
-      <c r="F539">
-        <v>7.0895000000000001</v>
-      </c>
-      <c r="G539">
-        <v>25</v>
-      </c>
-      <c r="H539">
-        <v>12.5</v>
-      </c>
-      <c r="I539">
-        <v>25</v>
-      </c>
-      <c r="J539">
-        <v>0</v>
-      </c>
-      <c r="K539">
-        <v>2</v>
-      </c>
-      <c r="L539">
-        <v>25</v>
-      </c>
-      <c r="M539">
-        <v>12.5</v>
-      </c>
-      <c r="N539">
-        <v>28</v>
-      </c>
-      <c r="O539">
-        <v>5.7041179779999999E-2</v>
-      </c>
-    </row>
-    <row r="540" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A540">
-        <v>0.59</v>
-      </c>
-      <c r="B540">
-        <v>2.1</v>
-      </c>
-      <c r="C540">
-        <v>-1</v>
-      </c>
-      <c r="D540">
-        <v>25</v>
-      </c>
-      <c r="E540">
-        <v>19.588999999999999</v>
-      </c>
-      <c r="F540">
-        <v>7.0895000000000001</v>
-      </c>
-      <c r="G540">
-        <v>25</v>
-      </c>
-      <c r="H540">
-        <v>12.5</v>
-      </c>
-      <c r="I540">
-        <v>25</v>
-      </c>
-      <c r="J540">
-        <v>0</v>
-      </c>
-      <c r="K540">
-        <v>2</v>
-      </c>
-      <c r="L540">
-        <v>25</v>
-      </c>
-      <c r="M540">
-        <v>25</v>
-      </c>
-      <c r="N540">
-        <v>116</v>
-      </c>
-      <c r="O540">
-        <v>5.9078364770000003E-2</v>
-      </c>
-    </row>
-    <row r="541" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A541">
-        <v>0.59</v>
-      </c>
-      <c r="B541">
-        <v>2.1</v>
-      </c>
-      <c r="C541">
-        <v>-1</v>
-      </c>
-      <c r="D541">
-        <v>25</v>
-      </c>
-      <c r="E541">
-        <v>19.588999999999999</v>
-      </c>
-      <c r="F541">
-        <v>7.0895000000000001</v>
-      </c>
-      <c r="G541">
-        <v>25</v>
-      </c>
-      <c r="H541">
-        <v>12.5</v>
-      </c>
-      <c r="I541">
-        <v>25</v>
-      </c>
-      <c r="J541">
-        <v>0</v>
-      </c>
-      <c r="K541">
-        <v>2</v>
-      </c>
-      <c r="L541">
-        <v>25</v>
-      </c>
-      <c r="M541">
-        <v>37.5</v>
-      </c>
-      <c r="N541">
-        <v>206</v>
-      </c>
-      <c r="O541">
         <v>4.6628900930000002E-2</v>
       </c>
     </row>
@@ -26911,6 +26875,7 @@
     <sortCondition ref="L366:L445"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -26919,7 +26884,7 @@
   <sheetPr filterMode="1"/>
   <dimension ref="A1:O361"/>
   <sheetViews>
-    <sheetView topLeftCell="A351" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C372" sqref="C372"/>
     </sheetView>
   </sheetViews>
@@ -42376,7 +42341,7 @@
         <v>16</v>
       </c>
       <c r="O322">
-        <f t="shared" ref="O322:O385" si="5">N322/(PI()*M322^2)</f>
+        <f t="shared" ref="O322:O361" si="5">N322/(PI()*M322^2)</f>
         <v>1.2732395447351627E-2</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Ball - Yang - Analysis: cubic zirconia distribution
appending sapphire ball version of same simulation
</commit_message>
<xml_diff>
--- a/Geometry/Ball/Papers/yang.xlsx
+++ b/Geometry/Ball/Papers/yang.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="25">
   <si>
     <t xml:space="preserve"> lens half submerged in channel medium above channel</t>
   </si>
@@ -705,7 +705,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -812,11 +811,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="156019904"/>
-        <c:axId val="156020464"/>
+        <c:axId val="63885216"/>
+        <c:axId val="63885776"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="156019904"/>
+        <c:axId val="63885216"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -873,12 +872,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="156020464"/>
+        <c:crossAx val="63885776"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="156020464"/>
+        <c:axId val="63885776"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -935,7 +934,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="156019904"/>
+        <c:crossAx val="63885216"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1043,7 +1042,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -1152,11 +1150,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="156022704"/>
-        <c:axId val="156023264"/>
+        <c:axId val="63888016"/>
+        <c:axId val="63888576"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="156022704"/>
+        <c:axId val="63888016"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1213,12 +1211,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="156023264"/>
+        <c:crossAx val="63888576"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="156023264"/>
+        <c:axId val="63888576"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1275,7 +1273,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="156022704"/>
+        <c:crossAx val="63888016"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2764,10 +2762,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:P537"/>
+  <dimension ref="A1:P530"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A464" workbookViewId="0">
-      <selection activeCell="M492" sqref="M492:P492"/>
+    <sheetView tabSelected="1" topLeftCell="A480" workbookViewId="0">
+      <selection activeCell="D492" sqref="D492"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -23562,7 +23560,7 @@
         <v>1.5844772159999999E-2</v>
       </c>
       <c r="P468" s="1">
-        <f t="shared" ref="P468:P474" si="5">(N468-N467)/(PI()*(M468^2-M467^2))</f>
+        <f t="shared" ref="P468:P473" si="5">(N468-N467)/(PI()*(M468^2-M467^2))</f>
         <v>1.711233948124059E-2</v>
       </c>
     </row>
@@ -24844,6 +24842,9 @@
       <c r="O494" s="4" t="s">
         <v>14</v>
       </c>
+      <c r="P494" s="4" t="s">
+        <v>24</v>
+      </c>
     </row>
     <row r="495" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A495">
@@ -24873,7 +24874,7 @@
       <c r="I495">
         <v>25</v>
       </c>
-      <c r="J495">
+      <c r="J495" s="1">
         <v>0</v>
       </c>
       <c r="K495">
@@ -24882,13 +24883,17 @@
       <c r="L495">
         <v>25</v>
       </c>
-      <c r="M495">
+      <c r="M495" s="1">
         <v>12.5</v>
       </c>
-      <c r="N495">
+      <c r="N495" s="1">
         <v>28</v>
       </c>
-      <c r="O495">
+      <c r="O495" s="1">
+        <v>5.7041179779999999E-2</v>
+      </c>
+      <c r="P495" s="1">
+        <f>O495</f>
         <v>5.7041179779999999E-2</v>
       </c>
     </row>
@@ -24920,7 +24925,7 @@
       <c r="I496">
         <v>25</v>
       </c>
-      <c r="J496">
+      <c r="J496" s="1">
         <v>0</v>
       </c>
       <c r="K496">
@@ -24929,17 +24934,21 @@
       <c r="L496">
         <v>25</v>
       </c>
-      <c r="M496">
-        <v>25</v>
-      </c>
-      <c r="N496">
+      <c r="M496" s="1">
+        <v>25</v>
+      </c>
+      <c r="N496" s="1">
         <v>116</v>
       </c>
-      <c r="O496">
+      <c r="O496" s="1">
         <v>5.9078364770000003E-2</v>
       </c>
-    </row>
-    <row r="497" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P496" s="1">
+        <f>(N496-N495)/(PI()*(M496^2-M495^2))</f>
+        <v>5.9757375966236967E-2</v>
+      </c>
+    </row>
+    <row r="497" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A497">
         <v>0.59</v>
       </c>
@@ -24967,7 +24976,7 @@
       <c r="I497">
         <v>25</v>
       </c>
-      <c r="J497">
+      <c r="J497" s="1">
         <v>0</v>
       </c>
       <c r="K497">
@@ -24976,17 +24985,21 @@
       <c r="L497">
         <v>25</v>
       </c>
-      <c r="M497">
+      <c r="M497" s="1">
         <v>37.5</v>
       </c>
-      <c r="N497">
+      <c r="N497" s="1">
         <v>206</v>
       </c>
-      <c r="O497">
+      <c r="O497" s="1">
         <v>4.6628900930000002E-2</v>
       </c>
-    </row>
-    <row r="498" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P497" s="1">
+        <f t="shared" ref="P497:P503" si="8">(N497-N496)/(PI()*(M497^2-M496^2))</f>
+        <v>3.6669298888372691E-2</v>
+      </c>
+    </row>
+    <row r="498" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A498">
         <v>0.59</v>
       </c>
@@ -25014,7 +25027,7 @@
       <c r="I498">
         <v>25</v>
       </c>
-      <c r="J498">
+      <c r="J498" s="1">
         <v>0</v>
       </c>
       <c r="K498">
@@ -25023,17 +25036,21 @@
       <c r="L498">
         <v>25</v>
       </c>
-      <c r="M498">
+      <c r="M498" s="1">
         <v>50</v>
       </c>
-      <c r="N498">
+      <c r="N498" s="1">
         <v>332</v>
       </c>
-      <c r="O498">
+      <c r="O498" s="1">
         <v>4.2271588589999999E-2</v>
       </c>
-    </row>
-    <row r="499" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P498" s="1">
+        <f t="shared" si="8"/>
+        <v>3.6669298888372691E-2</v>
+      </c>
+    </row>
+    <row r="499" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A499">
         <v>0.59</v>
       </c>
@@ -25061,7 +25078,7 @@
       <c r="I499">
         <v>25</v>
       </c>
-      <c r="J499">
+      <c r="J499" s="1">
         <v>0</v>
       </c>
       <c r="K499">
@@ -25070,17 +25087,21 @@
       <c r="L499">
         <v>25</v>
       </c>
-      <c r="M499">
+      <c r="M499" s="1">
         <v>62.5</v>
       </c>
-      <c r="N499">
+      <c r="N499" s="1">
         <v>362</v>
       </c>
-      <c r="O499">
+      <c r="O499" s="1">
         <v>2.9498438679999999E-2</v>
       </c>
-    </row>
-    <row r="500" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P499" s="1">
+        <f t="shared" si="8"/>
+        <v>6.7906109052542005E-3</v>
+      </c>
+    </row>
+    <row r="500" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A500">
         <v>0.59</v>
       </c>
@@ -25108,7 +25129,7 @@
       <c r="I500">
         <v>25</v>
       </c>
-      <c r="J500">
+      <c r="J500" s="1">
         <v>0</v>
       </c>
       <c r="K500">
@@ -25117,17 +25138,21 @@
       <c r="L500">
         <v>25</v>
       </c>
-      <c r="M500">
-        <v>75</v>
-      </c>
-      <c r="N500">
+      <c r="M500" s="1">
+        <v>75</v>
+      </c>
+      <c r="N500" s="1">
         <v>364</v>
       </c>
-      <c r="O500">
+      <c r="O500" s="1">
         <v>2.059820381E-2</v>
       </c>
-    </row>
-    <row r="501" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P500" s="1">
+        <f t="shared" si="8"/>
+        <v>3.7039695846841097E-4</v>
+      </c>
+    </row>
+    <row r="501" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A501">
         <v>0.59</v>
       </c>
@@ -25155,7 +25180,7 @@
       <c r="I501">
         <v>25</v>
       </c>
-      <c r="J501">
+      <c r="J501" s="1">
         <v>0</v>
       </c>
       <c r="K501">
@@ -25164,17 +25189,21 @@
       <c r="L501">
         <v>25</v>
       </c>
-      <c r="M501">
+      <c r="M501" s="1">
         <v>87.5</v>
       </c>
-      <c r="N501">
+      <c r="N501" s="1">
         <v>366</v>
       </c>
-      <c r="O501">
+      <c r="O501" s="1">
         <v>1.521652463E-2</v>
       </c>
-    </row>
-    <row r="502" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P501" s="1">
+        <f t="shared" si="8"/>
+        <v>3.1341281101173233E-4</v>
+      </c>
+    </row>
+    <row r="502" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A502">
         <v>0.59</v>
       </c>
@@ -25202,7 +25231,7 @@
       <c r="I502">
         <v>25</v>
       </c>
-      <c r="J502">
+      <c r="J502" s="1">
         <v>0</v>
       </c>
       <c r="K502">
@@ -25211,17 +25240,21 @@
       <c r="L502">
         <v>25</v>
       </c>
-      <c r="M502">
+      <c r="M502" s="1">
         <v>100</v>
       </c>
-      <c r="N502">
+      <c r="N502" s="1">
         <v>366</v>
       </c>
-      <c r="O502">
+      <c r="O502" s="1">
         <v>1.1650151669999999E-2</v>
       </c>
-    </row>
-    <row r="503" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P502" s="1">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="503" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A503">
         <v>0.59</v>
       </c>
@@ -25249,7 +25282,7 @@
       <c r="I503">
         <v>25</v>
       </c>
-      <c r="J503">
+      <c r="J503" s="1">
         <v>0</v>
       </c>
       <c r="K503">
@@ -25258,17 +25291,21 @@
       <c r="L503">
         <v>25</v>
       </c>
-      <c r="M503">
+      <c r="M503" s="1">
         <v>112.5</v>
       </c>
-      <c r="N503">
+      <c r="N503" s="1">
         <v>369</v>
       </c>
-      <c r="O503">
+      <c r="O503" s="1">
         <v>9.2805093999999994E-3</v>
       </c>
-    </row>
-    <row r="504" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P503" s="1">
+        <f t="shared" si="8"/>
+        <v>3.5950293027816363E-4</v>
+      </c>
+    </row>
+    <row r="504" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A504">
         <v>0.59</v>
       </c>
@@ -25296,26 +25333,30 @@
       <c r="I504">
         <v>25</v>
       </c>
-      <c r="J504">
-        <v>0</v>
+      <c r="J504" s="1">
+        <v>50</v>
       </c>
       <c r="K504">
         <v>2</v>
       </c>
       <c r="L504">
-        <v>25</v>
-      </c>
-      <c r="M504">
+        <v>75</v>
+      </c>
+      <c r="M504" s="1">
         <v>12.5</v>
       </c>
-      <c r="N504">
-        <v>28</v>
-      </c>
-      <c r="O504">
-        <v>5.7041179779999999E-2</v>
-      </c>
-    </row>
-    <row r="505" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="N504" s="1">
+        <v>3</v>
+      </c>
+      <c r="O504" s="1">
+        <v>6.1115549700000004E-3</v>
+      </c>
+      <c r="P504" s="1">
+        <f>O504</f>
+        <v>6.1115549700000004E-3</v>
+      </c>
+    </row>
+    <row r="505" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A505">
         <v>0.59</v>
       </c>
@@ -25343,7 +25384,7 @@
       <c r="I505">
         <v>25</v>
       </c>
-      <c r="J505">
+      <c r="J505" s="1">
         <v>50</v>
       </c>
       <c r="K505">
@@ -25352,17 +25393,21 @@
       <c r="L505">
         <v>75</v>
       </c>
-      <c r="M505">
-        <v>12.5</v>
-      </c>
-      <c r="N505">
-        <v>3</v>
-      </c>
-      <c r="O505">
-        <v>6.1115549700000004E-3</v>
-      </c>
-    </row>
-    <row r="506" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="M505" s="1">
+        <v>25</v>
+      </c>
+      <c r="N505" s="1">
+        <v>31</v>
+      </c>
+      <c r="O505" s="1">
+        <v>1.5788183689999999E-2</v>
+      </c>
+      <c r="P505" s="1">
+        <f>(N505-N504)/(PI()*(M505^2-M504^2))</f>
+        <v>1.9013710534711764E-2</v>
+      </c>
+    </row>
+    <row r="506" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A506">
         <v>0.59</v>
       </c>
@@ -25390,7 +25435,7 @@
       <c r="I506">
         <v>25</v>
       </c>
-      <c r="J506">
+      <c r="J506" s="1">
         <v>50</v>
       </c>
       <c r="K506">
@@ -25399,17 +25444,21 @@
       <c r="L506">
         <v>75</v>
       </c>
-      <c r="M506">
-        <v>25</v>
-      </c>
-      <c r="N506">
-        <v>31</v>
-      </c>
-      <c r="O506">
-        <v>1.5788183689999999E-2</v>
-      </c>
-    </row>
-    <row r="507" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="M506" s="1">
+        <v>37.5</v>
+      </c>
+      <c r="N506" s="1">
+        <v>67</v>
+      </c>
+      <c r="O506" s="1">
+        <v>1.516571049E-2</v>
+      </c>
+      <c r="P506" s="1">
+        <f t="shared" ref="P506:P512" si="9">(N506-N505)/(PI()*(M506^2-M505^2))</f>
+        <v>1.4667719555349075E-2</v>
+      </c>
+    </row>
+    <row r="507" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A507">
         <v>0.59</v>
       </c>
@@ -25437,7 +25486,7 @@
       <c r="I507">
         <v>25</v>
       </c>
-      <c r="J507">
+      <c r="J507" s="1">
         <v>50</v>
       </c>
       <c r="K507">
@@ -25446,17 +25495,21 @@
       <c r="L507">
         <v>75</v>
       </c>
-      <c r="M507">
-        <v>37.5</v>
-      </c>
-      <c r="N507">
-        <v>67</v>
-      </c>
-      <c r="O507">
-        <v>1.516571049E-2</v>
-      </c>
-    </row>
-    <row r="508" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="M507" s="1">
+        <v>50</v>
+      </c>
+      <c r="N507" s="1">
+        <v>98</v>
+      </c>
+      <c r="O507" s="1">
+        <v>1.2477758070000001E-2</v>
+      </c>
+      <c r="P507" s="1">
+        <f t="shared" si="9"/>
+        <v>9.0218116312662956E-3</v>
+      </c>
+    </row>
+    <row r="508" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A508">
         <v>0.59</v>
       </c>
@@ -25484,7 +25537,7 @@
       <c r="I508">
         <v>25</v>
       </c>
-      <c r="J508">
+      <c r="J508" s="1">
         <v>50</v>
       </c>
       <c r="K508">
@@ -25493,17 +25546,21 @@
       <c r="L508">
         <v>75</v>
       </c>
-      <c r="M508">
-        <v>50</v>
-      </c>
-      <c r="N508">
-        <v>98</v>
-      </c>
-      <c r="O508">
-        <v>1.2477758070000001E-2</v>
-      </c>
-    </row>
-    <row r="509" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="M508" s="1">
+        <v>62.5</v>
+      </c>
+      <c r="N508" s="1">
+        <v>153</v>
+      </c>
+      <c r="O508" s="1">
+        <v>1.246757215E-2</v>
+      </c>
+      <c r="P508" s="1">
+        <f t="shared" si="9"/>
+        <v>1.2449453326299369E-2</v>
+      </c>
+    </row>
+    <row r="509" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A509">
         <v>0.59</v>
       </c>
@@ -25531,7 +25588,7 @@
       <c r="I509">
         <v>25</v>
       </c>
-      <c r="J509">
+      <c r="J509" s="1">
         <v>50</v>
       </c>
       <c r="K509">
@@ -25540,17 +25597,21 @@
       <c r="L509">
         <v>75</v>
       </c>
-      <c r="M509">
-        <v>62.5</v>
-      </c>
-      <c r="N509">
-        <v>153</v>
-      </c>
-      <c r="O509">
-        <v>1.246757215E-2</v>
-      </c>
-    </row>
-    <row r="510" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="M509" s="1">
+        <v>75</v>
+      </c>
+      <c r="N509" s="1">
+        <v>214</v>
+      </c>
+      <c r="O509" s="1">
+        <v>1.2109933010000001E-2</v>
+      </c>
+      <c r="P509" s="1">
+        <f t="shared" si="9"/>
+        <v>1.1297107233286535E-2</v>
+      </c>
+    </row>
+    <row r="510" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A510">
         <v>0.59</v>
       </c>
@@ -25578,7 +25639,7 @@
       <c r="I510">
         <v>25</v>
       </c>
-      <c r="J510">
+      <c r="J510" s="1">
         <v>50</v>
       </c>
       <c r="K510">
@@ -25587,17 +25648,21 @@
       <c r="L510">
         <v>75</v>
       </c>
-      <c r="M510">
-        <v>75</v>
-      </c>
-      <c r="N510">
-        <v>214</v>
-      </c>
-      <c r="O510">
-        <v>1.2109933010000001E-2</v>
-      </c>
-    </row>
-    <row r="511" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="M510" s="1">
+        <v>87.5</v>
+      </c>
+      <c r="N510" s="1">
+        <v>288</v>
+      </c>
+      <c r="O510" s="1">
+        <v>1.197365873E-2</v>
+      </c>
+      <c r="P510" s="1">
+        <f t="shared" si="9"/>
+        <v>1.1596274007434097E-2</v>
+      </c>
+    </row>
+    <row r="511" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A511">
         <v>0.59</v>
       </c>
@@ -25625,7 +25690,7 @@
       <c r="I511">
         <v>25</v>
       </c>
-      <c r="J511">
+      <c r="J511" s="1">
         <v>50</v>
       </c>
       <c r="K511">
@@ -25634,17 +25699,21 @@
       <c r="L511">
         <v>75</v>
       </c>
-      <c r="M511">
-        <v>87.5</v>
-      </c>
-      <c r="N511">
-        <v>288</v>
-      </c>
-      <c r="O511">
-        <v>1.197365873E-2</v>
-      </c>
-    </row>
-    <row r="512" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="M511" s="1">
+        <v>100</v>
+      </c>
+      <c r="N511" s="1">
+        <v>345</v>
+      </c>
+      <c r="O511" s="1">
+        <v>1.0981700340000001E-2</v>
+      </c>
+      <c r="P511" s="1">
+        <f t="shared" si="9"/>
+        <v>7.7412964319897894E-3</v>
+      </c>
+    </row>
+    <row r="512" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A512">
         <v>0.59</v>
       </c>
@@ -25672,7 +25741,7 @@
       <c r="I512">
         <v>25</v>
       </c>
-      <c r="J512">
+      <c r="J512" s="1">
         <v>50</v>
       </c>
       <c r="K512">
@@ -25681,17 +25750,21 @@
       <c r="L512">
         <v>75</v>
       </c>
-      <c r="M512">
-        <v>100</v>
-      </c>
-      <c r="N512">
-        <v>345</v>
-      </c>
-      <c r="O512">
-        <v>1.0981700340000001E-2</v>
-      </c>
-    </row>
-    <row r="513" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="M512" s="1">
+        <v>112.5</v>
+      </c>
+      <c r="N512" s="1">
+        <v>361</v>
+      </c>
+      <c r="O512" s="1">
+        <v>9.0793059499999999E-3</v>
+      </c>
+      <c r="P512" s="1">
+        <f t="shared" si="9"/>
+        <v>1.9173489614835392E-3</v>
+      </c>
+    </row>
+    <row r="513" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A513">
         <v>0.59</v>
       </c>
@@ -25719,26 +25792,30 @@
       <c r="I513">
         <v>25</v>
       </c>
-      <c r="J513">
-        <v>50</v>
+      <c r="J513" s="1">
+        <v>100</v>
       </c>
       <c r="K513">
         <v>2</v>
       </c>
       <c r="L513">
-        <v>75</v>
-      </c>
-      <c r="M513">
-        <v>112.5</v>
-      </c>
-      <c r="N513">
-        <v>361</v>
-      </c>
-      <c r="O513">
-        <v>9.0793059499999999E-3</v>
-      </c>
-    </row>
-    <row r="514" spans="1:15" x14ac:dyDescent="0.3">
+        <v>125</v>
+      </c>
+      <c r="M513" s="1">
+        <v>12.5</v>
+      </c>
+      <c r="N513" s="1">
+        <v>1</v>
+      </c>
+      <c r="O513" s="1">
+        <v>2.03718499E-3</v>
+      </c>
+      <c r="P513" s="1">
+        <f>O513</f>
+        <v>2.03718499E-3</v>
+      </c>
+    </row>
+    <row r="514" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A514">
         <v>0.59</v>
       </c>
@@ -25766,26 +25843,30 @@
       <c r="I514">
         <v>25</v>
       </c>
-      <c r="J514">
-        <v>50</v>
+      <c r="J514" s="1">
+        <v>100</v>
       </c>
       <c r="K514">
         <v>2</v>
       </c>
       <c r="L514">
-        <v>75</v>
-      </c>
-      <c r="M514">
-        <v>12.5</v>
-      </c>
-      <c r="N514">
+        <v>125</v>
+      </c>
+      <c r="M514" s="1">
+        <v>25</v>
+      </c>
+      <c r="N514" s="1">
         <v>3</v>
       </c>
-      <c r="O514">
-        <v>6.1115549700000004E-3</v>
-      </c>
-    </row>
-    <row r="515" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="O514" s="1">
+        <v>1.5278887399999999E-3</v>
+      </c>
+      <c r="P514" s="1">
+        <f>(N514-N513)/(PI()*(M514^2-M513^2))</f>
+        <v>1.3581221810508401E-3</v>
+      </c>
+    </row>
+    <row r="515" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A515">
         <v>0.59</v>
       </c>
@@ -25813,7 +25894,7 @@
       <c r="I515">
         <v>25</v>
       </c>
-      <c r="J515">
+      <c r="J515" s="1">
         <v>100</v>
       </c>
       <c r="K515">
@@ -25822,17 +25903,21 @@
       <c r="L515">
         <v>125</v>
       </c>
-      <c r="M515">
-        <v>12.5</v>
-      </c>
-      <c r="N515">
-        <v>1</v>
-      </c>
-      <c r="O515">
-        <v>2.03718499E-3</v>
-      </c>
-    </row>
-    <row r="516" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="M515" s="1">
+        <v>37.5</v>
+      </c>
+      <c r="N515" s="1">
+        <v>16</v>
+      </c>
+      <c r="O515" s="1">
+        <v>3.6216622E-3</v>
+      </c>
+      <c r="P515" s="1">
+        <f t="shared" ref="P515:P521" si="10">(N515-N514)/(PI()*(M515^2-M514^2))</f>
+        <v>5.2966765060982772E-3</v>
+      </c>
+    </row>
+    <row r="516" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A516">
         <v>0.59</v>
       </c>
@@ -25860,7 +25945,7 @@
       <c r="I516">
         <v>25</v>
       </c>
-      <c r="J516">
+      <c r="J516" s="1">
         <v>100</v>
       </c>
       <c r="K516">
@@ -25869,17 +25954,21 @@
       <c r="L516">
         <v>125</v>
       </c>
-      <c r="M516">
-        <v>25</v>
-      </c>
-      <c r="N516">
-        <v>3</v>
-      </c>
-      <c r="O516">
-        <v>1.5278887399999999E-3</v>
-      </c>
-    </row>
-    <row r="517" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="M516" s="1">
+        <v>50</v>
+      </c>
+      <c r="N516" s="1">
+        <v>54</v>
+      </c>
+      <c r="O516" s="1">
+        <v>6.8754993399999997E-3</v>
+      </c>
+      <c r="P516" s="1">
+        <f t="shared" si="10"/>
+        <v>1.1058994902842557E-2</v>
+      </c>
+    </row>
+    <row r="517" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A517">
         <v>0.59</v>
       </c>
@@ -25907,7 +25996,7 @@
       <c r="I517">
         <v>25</v>
       </c>
-      <c r="J517">
+      <c r="J517" s="1">
         <v>100</v>
       </c>
       <c r="K517">
@@ -25916,17 +26005,21 @@
       <c r="L517">
         <v>125</v>
       </c>
-      <c r="M517">
-        <v>37.5</v>
-      </c>
-      <c r="N517">
-        <v>16</v>
-      </c>
-      <c r="O517">
-        <v>3.6216622E-3</v>
-      </c>
-    </row>
-    <row r="518" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="M517" s="1">
+        <v>62.5</v>
+      </c>
+      <c r="N517" s="1">
+        <v>81</v>
+      </c>
+      <c r="O517" s="1">
+        <v>6.6004793699999996E-3</v>
+      </c>
+      <c r="P517" s="1">
+        <f t="shared" si="10"/>
+        <v>6.1115498147287809E-3</v>
+      </c>
+    </row>
+    <row r="518" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A518">
         <v>0.59</v>
       </c>
@@ -25954,7 +26047,7 @@
       <c r="I518">
         <v>25</v>
       </c>
-      <c r="J518">
+      <c r="J518" s="1">
         <v>100</v>
       </c>
       <c r="K518">
@@ -25963,17 +26056,21 @@
       <c r="L518">
         <v>125</v>
       </c>
-      <c r="M518">
-        <v>50</v>
-      </c>
-      <c r="N518">
-        <v>54</v>
-      </c>
-      <c r="O518">
-        <v>6.8754993399999997E-3</v>
-      </c>
-    </row>
-    <row r="519" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="M518" s="1">
+        <v>75</v>
+      </c>
+      <c r="N518" s="1">
+        <v>104</v>
+      </c>
+      <c r="O518" s="1">
+        <v>5.8852010800000002E-3</v>
+      </c>
+      <c r="P518" s="1">
+        <f t="shared" si="10"/>
+        <v>4.259565022386726E-3</v>
+      </c>
+    </row>
+    <row r="519" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A519">
         <v>0.59</v>
       </c>
@@ -26001,7 +26098,7 @@
       <c r="I519">
         <v>25</v>
       </c>
-      <c r="J519">
+      <c r="J519" s="1">
         <v>100</v>
       </c>
       <c r="K519">
@@ -26010,17 +26107,21 @@
       <c r="L519">
         <v>125</v>
       </c>
-      <c r="M519">
-        <v>62.5</v>
-      </c>
-      <c r="N519">
-        <v>81</v>
-      </c>
-      <c r="O519">
-        <v>6.6004793699999996E-3</v>
-      </c>
-    </row>
-    <row r="520" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="M519" s="1">
+        <v>87.5</v>
+      </c>
+      <c r="N519" s="1">
+        <v>142</v>
+      </c>
+      <c r="O519" s="1">
+        <v>5.9036789500000004E-3</v>
+      </c>
+      <c r="P519" s="1">
+        <f t="shared" si="10"/>
+        <v>5.9548434092229147E-3</v>
+      </c>
+    </row>
+    <row r="520" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A520">
         <v>0.59</v>
       </c>
@@ -26048,7 +26149,7 @@
       <c r="I520">
         <v>25</v>
       </c>
-      <c r="J520">
+      <c r="J520" s="1">
         <v>100</v>
       </c>
       <c r="K520">
@@ -26057,17 +26158,21 @@
       <c r="L520">
         <v>125</v>
       </c>
-      <c r="M520">
-        <v>75</v>
-      </c>
-      <c r="N520">
-        <v>104</v>
-      </c>
-      <c r="O520">
-        <v>5.8852010800000002E-3</v>
-      </c>
-    </row>
-    <row r="521" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="M520" s="1">
+        <v>100</v>
+      </c>
+      <c r="N520" s="1">
+        <v>191</v>
+      </c>
+      <c r="O520" s="1">
+        <v>6.0797239600000001E-3</v>
+      </c>
+      <c r="P520" s="1">
+        <f t="shared" si="10"/>
+        <v>6.6547986871491171E-3</v>
+      </c>
+    </row>
+    <row r="521" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A521">
         <v>0.59</v>
       </c>
@@ -26095,7 +26200,7 @@
       <c r="I521">
         <v>25</v>
       </c>
-      <c r="J521">
+      <c r="J521" s="1">
         <v>100</v>
       </c>
       <c r="K521">
@@ -26104,17 +26209,21 @@
       <c r="L521">
         <v>125</v>
       </c>
-      <c r="M521">
-        <v>87.5</v>
-      </c>
-      <c r="N521">
-        <v>142</v>
-      </c>
-      <c r="O521">
-        <v>5.9036789500000004E-3</v>
-      </c>
-    </row>
-    <row r="522" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="M521" s="1">
+        <v>112.5</v>
+      </c>
+      <c r="N521" s="1">
+        <v>230</v>
+      </c>
+      <c r="O521" s="1">
+        <v>5.7845993599999999E-3</v>
+      </c>
+      <c r="P521" s="1">
+        <f t="shared" si="10"/>
+        <v>4.6735380936161267E-3</v>
+      </c>
+    </row>
+    <row r="522" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A522">
         <v>0.59</v>
       </c>
@@ -26142,26 +26251,30 @@
       <c r="I522">
         <v>25</v>
       </c>
-      <c r="J522">
-        <v>100</v>
+      <c r="J522" s="1">
+        <v>150</v>
       </c>
       <c r="K522">
         <v>2</v>
       </c>
       <c r="L522">
-        <v>125</v>
-      </c>
-      <c r="M522">
-        <v>100</v>
-      </c>
-      <c r="N522">
-        <v>191</v>
-      </c>
-      <c r="O522">
-        <v>6.0797239600000001E-3</v>
-      </c>
-    </row>
-    <row r="523" spans="1:15" x14ac:dyDescent="0.3">
+        <v>175</v>
+      </c>
+      <c r="M522" s="1">
+        <v>12.5</v>
+      </c>
+      <c r="N522" s="1">
+        <v>0</v>
+      </c>
+      <c r="O522" s="1">
+        <v>0</v>
+      </c>
+      <c r="P522" s="1">
+        <f>O522</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="523" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A523">
         <v>0.59</v>
       </c>
@@ -26189,26 +26302,30 @@
       <c r="I523">
         <v>25</v>
       </c>
-      <c r="J523">
-        <v>100</v>
+      <c r="J523" s="1">
+        <v>150</v>
       </c>
       <c r="K523">
         <v>2</v>
       </c>
       <c r="L523">
-        <v>125</v>
-      </c>
-      <c r="M523">
-        <v>112.5</v>
-      </c>
-      <c r="N523">
-        <v>230</v>
-      </c>
-      <c r="O523">
-        <v>5.7845993599999999E-3</v>
-      </c>
-    </row>
-    <row r="524" spans="1:15" x14ac:dyDescent="0.3">
+        <v>175</v>
+      </c>
+      <c r="M523" s="1">
+        <v>25</v>
+      </c>
+      <c r="N523" s="1">
+        <v>1</v>
+      </c>
+      <c r="O523" s="1">
+        <v>5.0929624000000003E-4</v>
+      </c>
+      <c r="P523" s="1">
+        <f>(N523-N522)/(PI()*(M523^2-M522^2))</f>
+        <v>6.7906109052542007E-4</v>
+      </c>
+    </row>
+    <row r="524" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A524">
         <v>0.59</v>
       </c>
@@ -26236,26 +26353,30 @@
       <c r="I524">
         <v>25</v>
       </c>
-      <c r="J524">
-        <v>100</v>
+      <c r="J524" s="1">
+        <v>150</v>
       </c>
       <c r="K524">
         <v>2</v>
       </c>
       <c r="L524">
-        <v>125</v>
-      </c>
-      <c r="M524">
-        <v>12.5</v>
-      </c>
-      <c r="N524">
-        <v>1</v>
-      </c>
-      <c r="O524">
-        <v>2.03718499E-3</v>
-      </c>
-    </row>
-    <row r="525" spans="1:15" x14ac:dyDescent="0.3">
+        <v>175</v>
+      </c>
+      <c r="M524" s="1">
+        <v>37.5</v>
+      </c>
+      <c r="N524" s="1">
+        <v>4</v>
+      </c>
+      <c r="O524" s="1">
+        <v>9.0541554999999999E-4</v>
+      </c>
+      <c r="P524" s="1">
+        <f t="shared" ref="P524:P530" si="11">(N524-N523)/(PI()*(M524^2-M523^2))</f>
+        <v>1.2223099629457563E-3</v>
+      </c>
+    </row>
+    <row r="525" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A525">
         <v>0.59</v>
       </c>
@@ -26283,7 +26404,7 @@
       <c r="I525">
         <v>25</v>
       </c>
-      <c r="J525">
+      <c r="J525" s="1">
         <v>150</v>
       </c>
       <c r="K525">
@@ -26292,17 +26413,21 @@
       <c r="L525">
         <v>175</v>
       </c>
-      <c r="M525">
-        <v>12.5</v>
-      </c>
-      <c r="N525">
-        <v>0</v>
-      </c>
-      <c r="O525">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="526" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="M525" s="1">
+        <v>50</v>
+      </c>
+      <c r="N525" s="1">
+        <v>12</v>
+      </c>
+      <c r="O525" s="1">
+        <v>1.5278887399999999E-3</v>
+      </c>
+      <c r="P525" s="1">
+        <f t="shared" si="11"/>
+        <v>2.328209453230012E-3</v>
+      </c>
+    </row>
+    <row r="526" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A526">
         <v>0.59</v>
       </c>
@@ -26330,7 +26455,7 @@
       <c r="I526">
         <v>25</v>
       </c>
-      <c r="J526">
+      <c r="J526" s="1">
         <v>150</v>
       </c>
       <c r="K526">
@@ -26339,17 +26464,21 @@
       <c r="L526">
         <v>175</v>
       </c>
-      <c r="M526">
-        <v>25</v>
-      </c>
-      <c r="N526">
-        <v>1</v>
-      </c>
-      <c r="O526">
-        <v>5.0929624000000003E-4</v>
-      </c>
-    </row>
-    <row r="527" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="M526" s="1">
+        <v>62.5</v>
+      </c>
+      <c r="N526" s="1">
+        <v>45</v>
+      </c>
+      <c r="O526" s="1">
+        <v>3.6669329799999999E-3</v>
+      </c>
+      <c r="P526" s="1">
+        <f t="shared" si="11"/>
+        <v>7.4696719957796209E-3</v>
+      </c>
+    </row>
+    <row r="527" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A527">
         <v>0.59</v>
       </c>
@@ -26377,7 +26506,7 @@
       <c r="I527">
         <v>25</v>
       </c>
-      <c r="J527">
+      <c r="J527" s="1">
         <v>150</v>
       </c>
       <c r="K527">
@@ -26386,17 +26515,21 @@
       <c r="L527">
         <v>175</v>
       </c>
-      <c r="M527">
-        <v>37.5</v>
-      </c>
-      <c r="N527">
-        <v>4</v>
-      </c>
-      <c r="O527">
-        <v>9.0541554999999999E-4</v>
-      </c>
-    </row>
-    <row r="528" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="M527" s="1">
+        <v>75</v>
+      </c>
+      <c r="N527" s="1">
+        <v>59</v>
+      </c>
+      <c r="O527" s="1">
+        <v>3.3387198400000001E-3</v>
+      </c>
+      <c r="P527" s="1">
+        <f t="shared" si="11"/>
+        <v>2.592778709278877E-3</v>
+      </c>
+    </row>
+    <row r="528" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A528">
         <v>0.59</v>
       </c>
@@ -26424,7 +26557,7 @@
       <c r="I528">
         <v>25</v>
       </c>
-      <c r="J528">
+      <c r="J528" s="1">
         <v>150</v>
       </c>
       <c r="K528">
@@ -26433,17 +26566,21 @@
       <c r="L528">
         <v>175</v>
       </c>
-      <c r="M528">
-        <v>50</v>
-      </c>
-      <c r="N528">
-        <v>12</v>
-      </c>
-      <c r="O528">
-        <v>1.5278887399999999E-3</v>
-      </c>
-    </row>
-    <row r="529" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="M528" s="1">
+        <v>87.5</v>
+      </c>
+      <c r="N528" s="1">
+        <v>77</v>
+      </c>
+      <c r="O528" s="1">
+        <v>3.2012907000000001E-3</v>
+      </c>
+      <c r="P528" s="1">
+        <f t="shared" si="11"/>
+        <v>2.8207152991055911E-3</v>
+      </c>
+    </row>
+    <row r="529" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A529">
         <v>0.59</v>
       </c>
@@ -26471,7 +26608,7 @@
       <c r="I529">
         <v>25</v>
       </c>
-      <c r="J529">
+      <c r="J529" s="1">
         <v>150</v>
       </c>
       <c r="K529">
@@ -26480,17 +26617,21 @@
       <c r="L529">
         <v>175</v>
       </c>
-      <c r="M529">
-        <v>62.5</v>
-      </c>
-      <c r="N529">
-        <v>45</v>
-      </c>
-      <c r="O529">
-        <v>3.6669329799999999E-3</v>
-      </c>
-    </row>
-    <row r="530" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="M529" s="1">
+        <v>100</v>
+      </c>
+      <c r="N529" s="1">
+        <v>96</v>
+      </c>
+      <c r="O529" s="1">
+        <v>3.0557774799999998E-3</v>
+      </c>
+      <c r="P529" s="1">
+        <f t="shared" si="11"/>
+        <v>2.5804321439965965E-3</v>
+      </c>
+    </row>
+    <row r="530" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A530">
         <v>0.59</v>
       </c>
@@ -26518,7 +26659,7 @@
       <c r="I530">
         <v>25</v>
       </c>
-      <c r="J530">
+      <c r="J530" s="1">
         <v>150</v>
       </c>
       <c r="K530">
@@ -26527,343 +26668,18 @@
       <c r="L530">
         <v>175</v>
       </c>
-      <c r="M530">
-        <v>75</v>
-      </c>
-      <c r="N530">
-        <v>59</v>
-      </c>
-      <c r="O530">
-        <v>3.3387198400000001E-3</v>
-      </c>
-    </row>
-    <row r="531" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A531">
-        <v>0.59</v>
-      </c>
-      <c r="B531">
-        <v>2.1</v>
-      </c>
-      <c r="C531">
-        <v>-1</v>
-      </c>
-      <c r="D531">
-        <v>25</v>
-      </c>
-      <c r="E531">
-        <v>19.588999999999999</v>
-      </c>
-      <c r="F531">
-        <v>7.0895000000000001</v>
-      </c>
-      <c r="G531">
-        <v>25</v>
-      </c>
-      <c r="H531">
-        <v>12.5</v>
-      </c>
-      <c r="I531">
-        <v>25</v>
-      </c>
-      <c r="J531">
-        <v>150</v>
-      </c>
-      <c r="K531">
-        <v>2</v>
-      </c>
-      <c r="L531">
-        <v>175</v>
-      </c>
-      <c r="M531">
-        <v>87.5</v>
-      </c>
-      <c r="N531">
-        <v>77</v>
-      </c>
-      <c r="O531">
-        <v>3.2012907000000001E-3</v>
-      </c>
-    </row>
-    <row r="532" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A532">
-        <v>0.59</v>
-      </c>
-      <c r="B532">
-        <v>2.1</v>
-      </c>
-      <c r="C532">
-        <v>-1</v>
-      </c>
-      <c r="D532">
-        <v>25</v>
-      </c>
-      <c r="E532">
-        <v>19.588999999999999</v>
-      </c>
-      <c r="F532">
-        <v>7.0895000000000001</v>
-      </c>
-      <c r="G532">
-        <v>25</v>
-      </c>
-      <c r="H532">
-        <v>12.5</v>
-      </c>
-      <c r="I532">
-        <v>25</v>
-      </c>
-      <c r="J532">
-        <v>150</v>
-      </c>
-      <c r="K532">
-        <v>2</v>
-      </c>
-      <c r="L532">
-        <v>175</v>
-      </c>
-      <c r="M532">
-        <v>100</v>
-      </c>
-      <c r="N532">
-        <v>96</v>
-      </c>
-      <c r="O532">
-        <v>3.0557774799999998E-3</v>
-      </c>
-    </row>
-    <row r="533" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A533">
-        <v>0.59</v>
-      </c>
-      <c r="B533">
-        <v>2.1</v>
-      </c>
-      <c r="C533">
-        <v>-1</v>
-      </c>
-      <c r="D533">
-        <v>25</v>
-      </c>
-      <c r="E533">
-        <v>19.588999999999999</v>
-      </c>
-      <c r="F533">
-        <v>7.0895000000000001</v>
-      </c>
-      <c r="G533">
-        <v>25</v>
-      </c>
-      <c r="H533">
-        <v>12.5</v>
-      </c>
-      <c r="I533">
-        <v>25</v>
-      </c>
-      <c r="J533">
-        <v>150</v>
-      </c>
-      <c r="K533">
-        <v>2</v>
-      </c>
-      <c r="L533">
-        <v>175</v>
-      </c>
-      <c r="M533">
+      <c r="M530" s="1">
         <v>112.5</v>
       </c>
-      <c r="N533">
+      <c r="N530" s="1">
         <v>117</v>
       </c>
-      <c r="O533">
+      <c r="O530" s="1">
         <v>2.9426005400000001E-3</v>
       </c>
-    </row>
-    <row r="534" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A534">
-        <v>0.59</v>
-      </c>
-      <c r="B534">
-        <v>2.1</v>
-      </c>
-      <c r="C534">
-        <v>-1</v>
-      </c>
-      <c r="D534">
-        <v>25</v>
-      </c>
-      <c r="E534">
-        <v>19.588999999999999</v>
-      </c>
-      <c r="F534">
-        <v>7.0895000000000001</v>
-      </c>
-      <c r="G534">
-        <v>25</v>
-      </c>
-      <c r="H534">
-        <v>12.5</v>
-      </c>
-      <c r="I534">
-        <v>25</v>
-      </c>
-      <c r="J534">
-        <v>150</v>
-      </c>
-      <c r="K534">
-        <v>2</v>
-      </c>
-      <c r="L534">
-        <v>175</v>
-      </c>
-      <c r="M534">
-        <v>12.5</v>
-      </c>
-      <c r="N534">
-        <v>0</v>
-      </c>
-      <c r="O534">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="535" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A535">
-        <v>0.59</v>
-      </c>
-      <c r="B535">
-        <v>2.1</v>
-      </c>
-      <c r="C535">
-        <v>-1</v>
-      </c>
-      <c r="D535">
-        <v>25</v>
-      </c>
-      <c r="E535">
-        <v>19.588999999999999</v>
-      </c>
-      <c r="F535">
-        <v>7.0895000000000001</v>
-      </c>
-      <c r="G535">
-        <v>25</v>
-      </c>
-      <c r="H535">
-        <v>12.5</v>
-      </c>
-      <c r="I535">
-        <v>25</v>
-      </c>
-      <c r="J535">
-        <v>0</v>
-      </c>
-      <c r="K535">
-        <v>2</v>
-      </c>
-      <c r="L535">
-        <v>25</v>
-      </c>
-      <c r="M535">
-        <v>12.5</v>
-      </c>
-      <c r="N535">
-        <v>28</v>
-      </c>
-      <c r="O535">
-        <v>5.7041179779999999E-2</v>
-      </c>
-    </row>
-    <row r="536" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A536">
-        <v>0.59</v>
-      </c>
-      <c r="B536">
-        <v>2.1</v>
-      </c>
-      <c r="C536">
-        <v>-1</v>
-      </c>
-      <c r="D536">
-        <v>25</v>
-      </c>
-      <c r="E536">
-        <v>19.588999999999999</v>
-      </c>
-      <c r="F536">
-        <v>7.0895000000000001</v>
-      </c>
-      <c r="G536">
-        <v>25</v>
-      </c>
-      <c r="H536">
-        <v>12.5</v>
-      </c>
-      <c r="I536">
-        <v>25</v>
-      </c>
-      <c r="J536">
-        <v>0</v>
-      </c>
-      <c r="K536">
-        <v>2</v>
-      </c>
-      <c r="L536">
-        <v>25</v>
-      </c>
-      <c r="M536">
-        <v>25</v>
-      </c>
-      <c r="N536">
-        <v>116</v>
-      </c>
-      <c r="O536">
-        <v>5.9078364770000003E-2</v>
-      </c>
-    </row>
-    <row r="537" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A537">
-        <v>0.59</v>
-      </c>
-      <c r="B537">
-        <v>2.1</v>
-      </c>
-      <c r="C537">
-        <v>-1</v>
-      </c>
-      <c r="D537">
-        <v>25</v>
-      </c>
-      <c r="E537">
-        <v>19.588999999999999</v>
-      </c>
-      <c r="F537">
-        <v>7.0895000000000001</v>
-      </c>
-      <c r="G537">
-        <v>25</v>
-      </c>
-      <c r="H537">
-        <v>12.5</v>
-      </c>
-      <c r="I537">
-        <v>25</v>
-      </c>
-      <c r="J537">
-        <v>0</v>
-      </c>
-      <c r="K537">
-        <v>2</v>
-      </c>
-      <c r="L537">
-        <v>25</v>
-      </c>
-      <c r="M537">
-        <v>37.5</v>
-      </c>
-      <c r="N537">
-        <v>206</v>
-      </c>
-      <c r="O537">
-        <v>4.6628900930000002E-2</v>
+      <c r="P530" s="1">
+        <f t="shared" si="11"/>
+        <v>2.5165205119471452E-3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Ball - Yang - Analysis: ray/area and rays
vs wd vs dr
</commit_message>
<xml_diff>
--- a/Geometry/Ball/Papers/yang.xlsx
+++ b/Geometry/Ball/Papers/yang.xlsx
@@ -811,11 +811,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="63885216"/>
-        <c:axId val="63885776"/>
+        <c:axId val="383028096"/>
+        <c:axId val="383028656"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="63885216"/>
+        <c:axId val="383028096"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -872,12 +872,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="63885776"/>
+        <c:crossAx val="383028656"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="63885776"/>
+        <c:axId val="383028656"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -934,7 +934,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="63885216"/>
+        <c:crossAx val="383028096"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1150,11 +1150,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="63888016"/>
-        <c:axId val="63888576"/>
+        <c:axId val="383030896"/>
+        <c:axId val="383031456"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="63888016"/>
+        <c:axId val="383030896"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1211,12 +1211,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="63888576"/>
+        <c:crossAx val="383031456"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="63888576"/>
+        <c:axId val="383031456"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1273,7 +1273,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="63888016"/>
+        <c:crossAx val="383030896"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2764,8 +2764,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P530"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A480" workbookViewId="0">
-      <selection activeCell="D492" sqref="D492"/>
+    <sheetView tabSelected="1" topLeftCell="A444" workbookViewId="0">
+      <selection activeCell="O495" sqref="O495"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2774,6 +2774,8 @@
     <col min="7" max="7" width="8.77734375" customWidth="1"/>
     <col min="9" max="9" width="11" customWidth="1"/>
     <col min="10" max="10" width="11.5546875" customWidth="1"/>
+    <col min="14" max="14" width="6.109375" customWidth="1"/>
+    <col min="15" max="15" width="10.6640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Ball - AWI/Yang Analysis: wd vs dr vs theta
AWI ball - better than baseline
Yang paper - not better than baeline

sanity check: baseline using lensless.inr produces same baseline as awi
ball
</commit_message>
<xml_diff>
--- a/Geometry/Ball/Papers/yang.xlsx
+++ b/Geometry/Ball/Papers/yang.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9576"/>
+    <workbookView minimized="1" xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9576"/>
   </bookViews>
   <sheets>
     <sheet name="yang" sheetId="1" r:id="rId1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="26">
   <si>
     <t xml:space="preserve"> lens half submerged in channel medium above channel</t>
   </si>
@@ -98,6 +98,9 @@
   </si>
   <si>
     <t>DISTRIBUTION</t>
+  </si>
+  <si>
+    <t>theta</t>
   </si>
 </sst>
 </file>
@@ -811,11 +814,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="383028096"/>
-        <c:axId val="383028656"/>
+        <c:axId val="168531824"/>
+        <c:axId val="168532384"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="383028096"/>
+        <c:axId val="168531824"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -872,12 +875,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="383028656"/>
+        <c:crossAx val="168532384"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="383028656"/>
+        <c:axId val="168532384"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -934,7 +937,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="383028096"/>
+        <c:crossAx val="168531824"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1150,11 +1153,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="383030896"/>
-        <c:axId val="383031456"/>
+        <c:axId val="168534624"/>
+        <c:axId val="168535184"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="383030896"/>
+        <c:axId val="168534624"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1211,12 +1214,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="383031456"/>
+        <c:crossAx val="168535184"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="383031456"/>
+        <c:axId val="168535184"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1273,7 +1276,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="383030896"/>
+        <c:crossAx val="168534624"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2762,10 +2765,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:P530"/>
+  <dimension ref="A1:Q530"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A444" workbookViewId="0">
-      <selection activeCell="O495" sqref="O495"/>
+    <sheetView tabSelected="1" topLeftCell="A454" workbookViewId="0">
+      <selection activeCell="L469" sqref="L469"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2773,7 +2776,8 @@
     <col min="1" max="1" width="11.77734375" customWidth="1"/>
     <col min="7" max="7" width="8.77734375" customWidth="1"/>
     <col min="9" max="9" width="11" customWidth="1"/>
-    <col min="10" max="10" width="11.5546875" customWidth="1"/>
+    <col min="10" max="10" width="36.88671875" customWidth="1"/>
+    <col min="12" max="12" width="32.109375" customWidth="1"/>
     <col min="14" max="14" width="6.109375" customWidth="1"/>
     <col min="15" max="15" width="10.6640625" customWidth="1"/>
   </cols>
@@ -24178,7 +24182,7 @@
         <v>3.333572626215699E-3</v>
       </c>
     </row>
-    <row r="481" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="481" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A481">
         <v>0.59</v>
       </c>
@@ -24229,7 +24233,7 @@
         <v>5.9548434092229147E-3</v>
       </c>
     </row>
-    <row r="482" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="482" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A482">
         <v>0.59</v>
       </c>
@@ -24280,7 +24284,7 @@
         <v>6.5189864690440328E-3</v>
       </c>
     </row>
-    <row r="483" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="483" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A483">
         <v>0.59</v>
       </c>
@@ -24331,7 +24335,7 @@
         <v>4.4338694734306844E-3</v>
       </c>
     </row>
-    <row r="484" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="484" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A484">
         <v>0.59</v>
       </c>
@@ -24382,7 +24386,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="485" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="485" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A485">
         <v>0.59</v>
       </c>
@@ -24433,7 +24437,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="486" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="486" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A486">
         <v>0.59</v>
       </c>
@@ -24484,7 +24488,7 @@
         <v>2.0371832715762603E-3</v>
       </c>
     </row>
-    <row r="487" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="487" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A487">
         <v>0.59</v>
       </c>
@@ -24535,7 +24539,7 @@
         <v>2.328209453230012E-3</v>
       </c>
     </row>
-    <row r="488" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="488" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A488">
         <v>0.59</v>
       </c>
@@ -24586,7 +24590,7 @@
         <v>7.0169646020960073E-3</v>
       </c>
     </row>
-    <row r="489" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="489" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A489">
         <v>0.59</v>
       </c>
@@ -24637,7 +24641,7 @@
         <v>2.592778709278877E-3</v>
       </c>
     </row>
-    <row r="490" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="490" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A490">
         <v>0.59</v>
       </c>
@@ -24688,7 +24692,7 @@
         <v>3.6042473266349219E-3</v>
       </c>
     </row>
-    <row r="491" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="491" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A491">
         <v>0.59</v>
       </c>
@@ -24739,7 +24743,7 @@
         <v>2.4446199258915126E-3</v>
       </c>
     </row>
-    <row r="492" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="492" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A492">
         <v>0.59</v>
       </c>
@@ -24790,7 +24794,7 @@
         <v>2.876023442225309E-3</v>
       </c>
     </row>
-    <row r="493" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="493" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A493" t="s">
         <v>22</v>
       </c>
@@ -24798,7 +24802,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="494" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="494" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A494" t="s">
         <v>1</v>
       </c>
@@ -24847,8 +24851,11 @@
       <c r="P494" s="4" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="495" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="Q494" s="4" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="495" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A495">
         <v>0.59</v>
       </c>
@@ -24898,8 +24905,12 @@
         <f>O495</f>
         <v>5.7041179779999999E-2</v>
       </c>
-    </row>
-    <row r="496" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="Q495">
+        <f>DEGREES(ACOS(1-(2*N495)/10000))</f>
+        <v>6.0664486091313643</v>
+      </c>
+    </row>
+    <row r="496" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A496">
         <v>0.59</v>
       </c>
@@ -24949,8 +24960,12 @@
         <f>(N496-N495)/(PI()*(M496^2-M495^2))</f>
         <v>5.9757375966236967E-2</v>
       </c>
-    </row>
-    <row r="497" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="Q496">
+        <f t="shared" ref="Q496:Q530" si="8">DEGREES(ACOS(1-(2*N496)/10000))</f>
+        <v>12.365875023113441</v>
+      </c>
+    </row>
+    <row r="497" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A497">
         <v>0.59</v>
       </c>
@@ -24997,11 +25012,15 @@
         <v>4.6628900930000002E-2</v>
       </c>
       <c r="P497" s="1">
-        <f t="shared" ref="P497:P503" si="8">(N497-N496)/(PI()*(M497^2-M496^2))</f>
+        <f t="shared" ref="P497:P503" si="9">(N497-N496)/(PI()*(M497^2-M496^2))</f>
         <v>3.6669298888372691E-2</v>
       </c>
-    </row>
-    <row r="498" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="Q497">
+        <f t="shared" si="8"/>
+        <v>16.503980742900492</v>
+      </c>
+    </row>
+    <row r="498" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A498">
         <v>0.59</v>
       </c>
@@ -25048,11 +25067,15 @@
         <v>4.2271588589999999E-2</v>
       </c>
       <c r="P498" s="1">
+        <f t="shared" si="9"/>
+        <v>3.6669298888372691E-2</v>
+      </c>
+      <c r="Q498">
         <f t="shared" si="8"/>
-        <v>3.6669298888372691E-2</v>
-      </c>
-    </row>
-    <row r="499" spans="1:16" x14ac:dyDescent="0.3">
+        <v>20.996870370524729</v>
+      </c>
+    </row>
+    <row r="499" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A499">
         <v>0.59</v>
       </c>
@@ -25099,11 +25122,15 @@
         <v>2.9498438679999999E-2</v>
       </c>
       <c r="P499" s="1">
+        <f t="shared" si="9"/>
+        <v>6.7906109052542005E-3</v>
+      </c>
+      <c r="Q499">
         <f t="shared" si="8"/>
-        <v>6.7906109052542005E-3</v>
-      </c>
-    </row>
-    <row r="500" spans="1:16" x14ac:dyDescent="0.3">
+        <v>21.936263130580741</v>
+      </c>
+    </row>
+    <row r="500" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A500">
         <v>0.59</v>
       </c>
@@ -25150,11 +25177,15 @@
         <v>2.059820381E-2</v>
       </c>
       <c r="P500" s="1">
+        <f t="shared" si="9"/>
+        <v>3.7039695846841097E-4</v>
+      </c>
+      <c r="Q500">
         <f t="shared" si="8"/>
-        <v>3.7039695846841097E-4</v>
-      </c>
-    </row>
-    <row r="501" spans="1:16" x14ac:dyDescent="0.3">
+        <v>21.997530437146043</v>
+      </c>
+    </row>
+    <row r="501" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A501">
         <v>0.59</v>
       </c>
@@ -25201,11 +25232,15 @@
         <v>1.521652463E-2</v>
       </c>
       <c r="P501" s="1">
+        <f t="shared" si="9"/>
+        <v>3.1341281101173233E-4</v>
+      </c>
+      <c r="Q501">
         <f t="shared" si="8"/>
-        <v>3.1341281101173233E-4</v>
-      </c>
-    </row>
-    <row r="502" spans="1:16" x14ac:dyDescent="0.3">
+        <v>22.058635997933226</v>
+      </c>
+    </row>
+    <row r="502" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A502">
         <v>0.59</v>
       </c>
@@ -25252,11 +25287,15 @@
         <v>1.1650151669999999E-2</v>
       </c>
       <c r="P502" s="1">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="Q502">
         <f t="shared" si="8"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="503" spans="1:16" x14ac:dyDescent="0.3">
+        <v>22.058635997933226</v>
+      </c>
+    </row>
+    <row r="503" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A503">
         <v>0.59</v>
       </c>
@@ -25303,11 +25342,15 @@
         <v>9.2805093999999994E-3</v>
       </c>
       <c r="P503" s="1">
+        <f t="shared" si="9"/>
+        <v>3.5950293027816363E-4</v>
+      </c>
+      <c r="Q503">
         <f t="shared" si="8"/>
-        <v>3.5950293027816363E-4</v>
-      </c>
-    </row>
-    <row r="504" spans="1:16" x14ac:dyDescent="0.3">
+        <v>22.149993999158106</v>
+      </c>
+    </row>
+    <row r="504" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A504">
         <v>0.59</v>
       </c>
@@ -25357,8 +25400,12 @@
         <f>O504</f>
         <v>6.1115549700000004E-3</v>
       </c>
-    </row>
-    <row r="505" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="Q504">
+        <f t="shared" si="8"/>
+        <v>1.9848832761193831</v>
+      </c>
+    </row>
+    <row r="505" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A505">
         <v>0.59</v>
       </c>
@@ -25408,8 +25455,12 @@
         <f>(N505-N504)/(PI()*(M505^2-M504^2))</f>
         <v>1.9013710534711764E-2</v>
       </c>
-    </row>
-    <row r="506" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="Q505">
+        <f t="shared" si="8"/>
+        <v>6.3834890237534783</v>
+      </c>
+    </row>
+    <row r="506" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A506">
         <v>0.59</v>
       </c>
@@ -25456,11 +25507,15 @@
         <v>1.516571049E-2</v>
       </c>
       <c r="P506" s="1">
-        <f t="shared" ref="P506:P512" si="9">(N506-N505)/(PI()*(M506^2-M505^2))</f>
+        <f t="shared" ref="P506:P512" si="10">(N506-N505)/(PI()*(M506^2-M505^2))</f>
         <v>1.4667719555349075E-2</v>
       </c>
-    </row>
-    <row r="507" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="Q506">
+        <f t="shared" si="8"/>
+        <v>9.3902290831924358</v>
+      </c>
+    </row>
+    <row r="507" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A507">
         <v>0.59</v>
       </c>
@@ -25507,11 +25562,15 @@
         <v>1.2477758070000001E-2</v>
       </c>
       <c r="P507" s="1">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>9.0218116312662956E-3</v>
       </c>
-    </row>
-    <row r="508" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="Q507">
+        <f t="shared" si="8"/>
+        <v>11.362596283942178</v>
+      </c>
+    </row>
+    <row r="508" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A508">
         <v>0.59</v>
       </c>
@@ -25558,11 +25617,15 @@
         <v>1.246757215E-2</v>
       </c>
       <c r="P508" s="1">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>1.2449453326299369E-2</v>
       </c>
-    </row>
-    <row r="509" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="Q508">
+        <f t="shared" si="8"/>
+        <v>14.210588385318809</v>
+      </c>
+    </row>
+    <row r="509" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A509">
         <v>0.59</v>
       </c>
@@ -25609,11 +25672,15 @@
         <v>1.2109933010000001E-2</v>
       </c>
       <c r="P509" s="1">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>1.1297107233286535E-2</v>
       </c>
-    </row>
-    <row r="510" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="Q509">
+        <f t="shared" si="8"/>
+        <v>16.823672215473991</v>
+      </c>
+    </row>
+    <row r="510" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A510">
         <v>0.59</v>
       </c>
@@ -25660,11 +25727,15 @@
         <v>1.197365873E-2</v>
       </c>
       <c r="P510" s="1">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>1.1596274007434097E-2</v>
       </c>
-    </row>
-    <row r="511" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="Q510">
+        <f t="shared" si="8"/>
+        <v>19.541408127043887</v>
+      </c>
+    </row>
+    <row r="511" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A511">
         <v>0.59</v>
       </c>
@@ -25711,11 +25782,15 @@
         <v>1.0981700340000001E-2</v>
       </c>
       <c r="P511" s="1">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>7.7412964319897894E-3</v>
       </c>
-    </row>
-    <row r="512" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="Q511">
+        <f t="shared" si="8"/>
+        <v>21.408762929275898</v>
+      </c>
+    </row>
+    <row r="512" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A512">
         <v>0.59</v>
       </c>
@@ -25762,11 +25837,15 @@
         <v>9.0793059499999999E-3</v>
       </c>
       <c r="P512" s="1">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>1.9173489614835392E-3</v>
       </c>
-    </row>
-    <row r="513" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="Q512">
+        <f t="shared" si="8"/>
+        <v>21.905568397782247</v>
+      </c>
+    </row>
+    <row r="513" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A513">
         <v>0.59</v>
       </c>
@@ -25816,8 +25895,12 @@
         <f>O513</f>
         <v>2.03718499E-3</v>
       </c>
-    </row>
-    <row r="514" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="Q513">
+        <f t="shared" si="8"/>
+        <v>1.1459346897142324</v>
+      </c>
+    </row>
+    <row r="514" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A514">
         <v>0.59</v>
       </c>
@@ -25867,8 +25950,12 @@
         <f>(N514-N513)/(PI()*(M514^2-M513^2))</f>
         <v>1.3581221810508401E-3</v>
       </c>
-    </row>
-    <row r="515" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="Q514">
+        <f t="shared" si="8"/>
+        <v>1.9848832761193831</v>
+      </c>
+    </row>
+    <row r="515" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A515">
         <v>0.59</v>
       </c>
@@ -25915,11 +26002,15 @@
         <v>3.6216622E-3</v>
       </c>
       <c r="P515" s="1">
-        <f t="shared" ref="P515:P521" si="10">(N515-N514)/(PI()*(M515^2-M514^2))</f>
+        <f t="shared" ref="P515:P521" si="11">(N515-N514)/(PI()*(M515^2-M514^2))</f>
         <v>5.2966765060982772E-3</v>
       </c>
-    </row>
-    <row r="516" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="Q515">
+        <f t="shared" si="8"/>
+        <v>4.5848855519117544</v>
+      </c>
+    </row>
+    <row r="516" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A516">
         <v>0.59</v>
       </c>
@@ -25966,11 +26057,15 @@
         <v>6.8754993399999997E-3</v>
       </c>
       <c r="P516" s="1">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>1.1058994902842557E-2</v>
       </c>
-    </row>
-    <row r="517" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="Q516">
+        <f t="shared" si="8"/>
+        <v>8.4283225817713667</v>
+      </c>
+    </row>
+    <row r="517" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A517">
         <v>0.59</v>
       </c>
@@ -26017,11 +26112,15 @@
         <v>6.6004793699999996E-3</v>
       </c>
       <c r="P517" s="1">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>6.1115498147287809E-3</v>
       </c>
-    </row>
-    <row r="518" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="Q517">
+        <f t="shared" si="8"/>
+        <v>10.327214181692757</v>
+      </c>
+    </row>
+    <row r="518" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A518">
         <v>0.59</v>
       </c>
@@ -26068,11 +26167,15 @@
         <v>5.8852010800000002E-3</v>
       </c>
       <c r="P518" s="1">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>4.259565022386726E-3</v>
       </c>
-    </row>
-    <row r="519" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="Q518">
+        <f t="shared" si="8"/>
+        <v>11.70644319260035</v>
+      </c>
+    </row>
+    <row r="519" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A519">
         <v>0.59</v>
       </c>
@@ -26119,11 +26222,15 @@
         <v>5.9036789500000004E-3</v>
       </c>
       <c r="P519" s="1">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>5.9548434092229147E-3</v>
       </c>
-    </row>
-    <row r="520" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="Q519">
+        <f t="shared" si="8"/>
+        <v>13.687685703748416</v>
+      </c>
+    </row>
+    <row r="520" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A520">
         <v>0.59</v>
       </c>
@@ -26170,11 +26277,15 @@
         <v>6.0797239600000001E-3</v>
       </c>
       <c r="P520" s="1">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>6.6547986871491171E-3</v>
       </c>
-    </row>
-    <row r="521" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="Q520">
+        <f t="shared" si="8"/>
+        <v>15.887720870984349</v>
+      </c>
+    </row>
+    <row r="521" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A521">
         <v>0.59</v>
       </c>
@@ -26221,11 +26332,15 @@
         <v>5.7845993599999999E-3</v>
       </c>
       <c r="P521" s="1">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>4.6735380936161267E-3</v>
       </c>
-    </row>
-    <row r="522" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="Q521">
+        <f t="shared" si="8"/>
+        <v>17.445987705778016</v>
+      </c>
+    </row>
+    <row r="522" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A522">
         <v>0.59</v>
       </c>
@@ -26275,8 +26390,12 @@
         <f>O522</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="523" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="Q522">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="523" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A523">
         <v>0.59</v>
       </c>
@@ -26326,8 +26445,12 @@
         <f>(N523-N522)/(PI()*(M523^2-M522^2))</f>
         <v>6.7906109052542007E-4</v>
       </c>
-    </row>
-    <row r="524" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="Q523">
+        <f t="shared" si="8"/>
+        <v>1.1459346897142324</v>
+      </c>
+    </row>
+    <row r="524" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A524">
         <v>0.59</v>
       </c>
@@ -26374,11 +26497,15 @@
         <v>9.0541554999999999E-4</v>
       </c>
       <c r="P524" s="1">
-        <f t="shared" ref="P524:P530" si="11">(N524-N523)/(PI()*(M524^2-M523^2))</f>
+        <f t="shared" ref="P524:P530" si="12">(N524-N523)/(PI()*(M524^2-M523^2))</f>
         <v>1.2223099629457563E-3</v>
       </c>
-    </row>
-    <row r="525" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="Q524">
+        <f t="shared" si="8"/>
+        <v>2.2919839967772129</v>
+      </c>
+    </row>
+    <row r="525" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A525">
         <v>0.59</v>
       </c>
@@ -26425,11 +26552,15 @@
         <v>1.5278887399999999E-3</v>
       </c>
       <c r="P525" s="1">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>2.328209453230012E-3</v>
       </c>
-    </row>
-    <row r="526" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="Q525">
+        <f t="shared" si="8"/>
+        <v>3.9703623896660907</v>
+      </c>
+    </row>
+    <row r="526" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A526">
         <v>0.59</v>
       </c>
@@ -26476,11 +26607,15 @@
         <v>3.6669329799999999E-3</v>
       </c>
       <c r="P526" s="1">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>7.4696719957796209E-3</v>
       </c>
-    </row>
-    <row r="527" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="Q526">
+        <f t="shared" si="8"/>
+        <v>7.6928124515598792</v>
+      </c>
+    </row>
+    <row r="527" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A527">
         <v>0.59</v>
       </c>
@@ -26527,11 +26662,15 @@
         <v>3.3387198400000001E-3</v>
       </c>
       <c r="P527" s="1">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>2.592778709278877E-3</v>
       </c>
-    </row>
-    <row r="528" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="Q527">
+        <f t="shared" si="8"/>
+        <v>8.8106229698453582</v>
+      </c>
+    </row>
+    <row r="528" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A528">
         <v>0.59</v>
       </c>
@@ -26578,11 +26717,15 @@
         <v>3.2012907000000001E-3</v>
       </c>
       <c r="P528" s="1">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>2.8207152991055911E-3</v>
       </c>
-    </row>
-    <row r="529" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="Q528">
+        <f t="shared" si="8"/>
+        <v>10.068317804800339</v>
+      </c>
+    </row>
+    <row r="529" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A529">
         <v>0.59</v>
       </c>
@@ -26629,11 +26772,15 @@
         <v>3.0557774799999998E-3</v>
       </c>
       <c r="P529" s="1">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>2.5804321439965965E-3</v>
       </c>
-    </row>
-    <row r="530" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="Q529">
+        <f t="shared" si="8"/>
+        <v>11.245676203848493</v>
+      </c>
+    </row>
+    <row r="530" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A530">
         <v>0.59</v>
       </c>
@@ -26680,8 +26827,12 @@
         <v>2.9426005400000001E-3</v>
       </c>
       <c r="P530" s="1">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>2.5165205119471452E-3</v>
+      </c>
+      <c r="Q530">
+        <f t="shared" si="8"/>
+        <v>12.419270599468586</v>
       </c>
     </row>
   </sheetData>

</xml_diff>